<commit_message>
Run code for all data for paper, change different things through meeting to avoid warnings
</commit_message>
<xml_diff>
--- a/experiments/thermal hydrolysis/data/BMP2.xlsx
+++ b/experiments/thermal hydrolysis/data/BMP2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="142">
   <si>
     <t>id</t>
   </si>
@@ -498,6 +498,15 @@
   </si>
   <si>
     <t>Add time.orig column with original times and adjusted time column to be the first time for each sampling day in both sheet = measurements and sheet = comp</t>
+  </si>
+  <si>
+    <t>22.02.2019</t>
+  </si>
+  <si>
+    <t>BMP2.xlxs</t>
+  </si>
+  <si>
+    <t>Change first B3 to B2 in comp data sheet for 07032017</t>
   </si>
 </sst>
 </file>
@@ -17698,8 +17707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17747,33 +17756,33 @@
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12">
-        <v>15022017</v>
+        <v>7032017</v>
       </c>
       <c r="C3" s="22">
-        <v>0.24390000000000001</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="D3" s="12">
-        <v>929</v>
+        <v>1104</v>
       </c>
       <c r="E3" s="12">
-        <v>929</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B4" s="12">
         <v>15022017</v>
       </c>
       <c r="C4" s="22">
-        <v>0.24390000000000001</v>
+        <v>0.46150000000000002</v>
       </c>
       <c r="D4" s="12">
-        <v>929</v>
+        <v>1016</v>
       </c>
       <c r="E4" s="12">
         <v>929</v>
@@ -17781,118 +17790,118 @@
     </row>
     <row r="5" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B5" s="12">
-        <v>15022017</v>
+        <v>16022017</v>
       </c>
       <c r="C5" s="22">
-        <v>0.24390000000000001</v>
+        <v>0.54430000000000001</v>
       </c>
       <c r="D5" s="12">
-        <v>929</v>
+        <v>1325</v>
       </c>
       <c r="E5" s="12">
-        <v>929</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B6" s="12">
-        <v>15022017</v>
+        <v>17022017</v>
       </c>
       <c r="C6" s="22">
-        <v>0.45279999999999998</v>
+        <v>0.58289999999999997</v>
       </c>
       <c r="D6" s="12">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="E6" s="12">
-        <v>929</v>
+        <v>854</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B7" s="12">
-        <v>15022017</v>
+        <v>18022017</v>
       </c>
       <c r="C7" s="22">
-        <v>0.46810000000000002</v>
+        <v>0.68540000000000001</v>
       </c>
       <c r="D7" s="12">
-        <v>935</v>
+        <v>1644</v>
       </c>
       <c r="E7" s="12">
-        <v>929</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B8" s="12">
-        <v>15022017</v>
+        <v>19022017</v>
       </c>
       <c r="C8" s="22">
-        <v>0.46810000000000002</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="D8" s="12">
-        <v>935</v>
+        <v>1634</v>
       </c>
       <c r="E8" s="12">
-        <v>929</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B9" s="12">
-        <v>15022017</v>
+        <v>20022017</v>
       </c>
       <c r="C9" s="22">
-        <v>0.48920000000000002</v>
+        <v>0.72419999999999995</v>
       </c>
       <c r="D9" s="12">
-        <v>941</v>
+        <v>1121</v>
       </c>
       <c r="E9" s="12">
-        <v>929</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B10" s="12">
-        <v>15022017</v>
+        <v>7032017</v>
       </c>
       <c r="C10" s="22">
-        <v>0.47639999999999999</v>
+        <v>0.67720000000000002</v>
       </c>
       <c r="D10" s="12">
-        <v>941</v>
+        <v>1104</v>
       </c>
       <c r="E10" s="12">
-        <v>929</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B11" s="12">
         <v>15022017</v>
       </c>
       <c r="C11" s="22">
-        <v>0.48559999999999998</v>
+        <v>0.4637</v>
       </c>
       <c r="D11" s="12">
-        <v>941</v>
+        <v>1016</v>
       </c>
       <c r="E11" s="12">
         <v>929</v>
@@ -17900,118 +17909,118 @@
     </row>
     <row r="12" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B12" s="12">
-        <v>15022017</v>
+        <v>16022017</v>
       </c>
       <c r="C12" s="22">
-        <v>0.39479999999999998</v>
+        <v>0.54830000000000001</v>
       </c>
       <c r="D12" s="12">
-        <v>949</v>
+        <v>1325</v>
       </c>
       <c r="E12" s="12">
-        <v>929</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B13" s="12">
-        <v>15022017</v>
+        <v>17022017</v>
       </c>
       <c r="C13" s="22">
-        <v>0.48620000000000002</v>
+        <v>0.58289999999999997</v>
       </c>
       <c r="D13" s="12">
-        <v>949</v>
+        <v>932</v>
       </c>
       <c r="E13" s="12">
-        <v>929</v>
+        <v>854</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B14" s="12">
-        <v>15022017</v>
+        <v>18022017</v>
       </c>
       <c r="C14" s="22">
-        <v>0.43290000000000001</v>
+        <v>0.68969999999999998</v>
       </c>
       <c r="D14" s="12">
-        <v>949</v>
+        <v>1644</v>
       </c>
       <c r="E14" s="12">
-        <v>929</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B15" s="12">
-        <v>15022017</v>
+        <v>19022017</v>
       </c>
       <c r="C15" s="22">
-        <v>0.37819999999999998</v>
+        <v>0.73329999999999995</v>
       </c>
       <c r="D15" s="12">
-        <v>956</v>
+        <v>1634</v>
       </c>
       <c r="E15" s="12">
-        <v>929</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B16" s="12">
-        <v>15022017</v>
+        <v>20022017</v>
       </c>
       <c r="C16" s="22">
-        <v>0.47149999999999997</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="D16" s="12">
-        <v>956</v>
+        <v>1121</v>
       </c>
       <c r="E16" s="12">
-        <v>929</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B17" s="12">
-        <v>15022017</v>
+        <v>7032017</v>
       </c>
       <c r="C17" s="22">
-        <v>0.47389999999999999</v>
+        <v>0.67369999999999997</v>
       </c>
       <c r="D17" s="12">
-        <v>956</v>
+        <v>1104</v>
       </c>
       <c r="E17" s="12">
-        <v>929</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B18" s="12">
         <v>15022017</v>
       </c>
       <c r="C18" s="22">
-        <v>0.37830000000000003</v>
+        <v>0.4597</v>
       </c>
       <c r="D18" s="12">
-        <v>1002</v>
+        <v>1016</v>
       </c>
       <c r="E18" s="12">
         <v>929</v>
@@ -18019,118 +18028,118 @@
     </row>
     <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B19" s="12">
-        <v>15022017</v>
+        <v>16022017</v>
       </c>
       <c r="C19" s="22">
-        <v>0.43480000000000002</v>
+        <v>0.55769999999999997</v>
       </c>
       <c r="D19" s="12">
-        <v>1002</v>
+        <v>1325</v>
       </c>
       <c r="E19" s="12">
-        <v>929</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B20" s="12">
-        <v>15022017</v>
+        <v>17022017</v>
       </c>
       <c r="C20" s="22">
-        <v>0.33289999999999997</v>
+        <v>0.60589999999999999</v>
       </c>
       <c r="D20" s="12">
-        <v>1002</v>
+        <v>932</v>
       </c>
       <c r="E20" s="12">
-        <v>929</v>
+        <v>854</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B21" s="12">
-        <v>15022017</v>
+        <v>18022017</v>
       </c>
       <c r="C21" s="22">
-        <v>0.24840000000000001</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="D21" s="12">
-        <v>1009</v>
+        <v>1644</v>
       </c>
       <c r="E21" s="12">
-        <v>929</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B22" s="12">
-        <v>15022017</v>
+        <v>19022017</v>
       </c>
       <c r="C22" s="22">
-        <v>0.44119999999999998</v>
+        <v>0.73550000000000004</v>
       </c>
       <c r="D22" s="12">
-        <v>1009</v>
+        <v>1634</v>
       </c>
       <c r="E22" s="12">
-        <v>929</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B23" s="12">
-        <v>15022017</v>
+        <v>20022017</v>
       </c>
       <c r="C23" s="22">
-        <v>0.4405</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="D23" s="12">
-        <v>1009</v>
+        <v>1121</v>
       </c>
       <c r="E23" s="12">
-        <v>929</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B24" s="12">
-        <v>15022017</v>
+        <v>7032017</v>
       </c>
       <c r="C24" s="22">
-        <v>0.46150000000000002</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="D24" s="12">
-        <v>1016</v>
+        <v>1108</v>
       </c>
       <c r="E24" s="12">
-        <v>929</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" s="12">
         <v>15022017</v>
       </c>
       <c r="C25" s="22">
-        <v>0.4637</v>
+        <v>0.40949999999999998</v>
       </c>
       <c r="D25" s="12">
-        <v>1016</v>
+        <v>1023</v>
       </c>
       <c r="E25" s="12">
         <v>929</v>
@@ -18138,19 +18147,19 @@
     </row>
     <row r="26" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="12">
-        <v>15022017</v>
+        <v>16022017</v>
       </c>
       <c r="C26" s="22">
-        <v>0.4597</v>
+        <v>0.51839999999999997</v>
       </c>
       <c r="D26" s="12">
-        <v>1016</v>
+        <v>1331</v>
       </c>
       <c r="E26" s="12">
-        <v>929</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -18158,81 +18167,81 @@
         <v>44</v>
       </c>
       <c r="B27" s="12">
-        <v>15022017</v>
+        <v>17022017</v>
       </c>
       <c r="C27" s="22">
-        <v>0.40949999999999998</v>
+        <v>0.5786</v>
       </c>
       <c r="D27" s="12">
-        <v>1023</v>
+        <v>937</v>
       </c>
       <c r="E27" s="12">
-        <v>929</v>
+        <v>854</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="12">
-        <v>15022017</v>
+        <v>18022017</v>
       </c>
       <c r="C28" s="22">
-        <v>0.4103</v>
+        <v>0.68379999999999996</v>
       </c>
       <c r="D28" s="12">
-        <v>1023</v>
+        <v>1650</v>
       </c>
       <c r="E28" s="12">
-        <v>929</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29" s="12">
-        <v>15022017</v>
+        <v>19022017</v>
       </c>
       <c r="C29" s="22">
-        <v>0.41399999999999998</v>
+        <v>0.72470000000000001</v>
       </c>
       <c r="D29" s="12">
-        <v>1023</v>
+        <v>1638</v>
       </c>
       <c r="E29" s="12">
-        <v>929</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B30" s="12">
-        <v>15022017</v>
+        <v>20022017</v>
       </c>
       <c r="C30" s="22">
-        <v>0.26229999999999998</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="D30" s="12">
-        <v>1029</v>
+        <v>1126</v>
       </c>
       <c r="E30" s="12">
-        <v>929</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B31" s="12">
         <v>15022017</v>
       </c>
       <c r="C31" s="22">
-        <v>0.251</v>
+        <v>0.4103</v>
       </c>
       <c r="D31" s="12">
-        <v>1029</v>
+        <v>1023</v>
       </c>
       <c r="E31" s="12">
         <v>929</v>
@@ -18240,152 +18249,152 @@
     </row>
     <row r="32" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>15022017</v>
+        <v>16022017</v>
       </c>
       <c r="C32" s="22">
-        <v>0.2432</v>
+        <v>0.51859999999999995</v>
       </c>
       <c r="D32" s="12">
-        <v>1029</v>
+        <v>1331</v>
       </c>
       <c r="E32" s="12">
-        <v>929</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
-        <v>15022017</v>
+        <v>17022017</v>
       </c>
       <c r="C33" s="22">
-        <v>0.51629999999999998</v>
+        <v>0.57920000000000005</v>
       </c>
       <c r="D33" s="12">
-        <v>1034</v>
+        <v>937</v>
       </c>
       <c r="E33" s="12">
-        <v>929</v>
+        <v>854</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34" s="12">
-        <v>15022017</v>
+        <v>18022017</v>
       </c>
       <c r="C34" s="22">
-        <v>0.51759999999999995</v>
+        <v>0.68289999999999995</v>
       </c>
       <c r="D34" s="12">
-        <v>1034</v>
+        <v>1650</v>
       </c>
       <c r="E34" s="12">
-        <v>929</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B35" s="12">
-        <v>15022017</v>
+        <v>19022017</v>
       </c>
       <c r="C35" s="22">
-        <v>0.51759999999999995</v>
+        <v>0.72470000000000001</v>
       </c>
       <c r="D35" s="12">
-        <v>1034</v>
+        <v>1638</v>
       </c>
       <c r="E35" s="12">
-        <v>929</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B36" s="12">
-        <v>16022017</v>
+        <v>20022017</v>
       </c>
       <c r="C36" s="22">
-        <v>0.39710000000000001</v>
+        <v>0.71330000000000005</v>
       </c>
       <c r="D36" s="12">
-        <v>1344</v>
+        <v>1126</v>
       </c>
       <c r="E36" s="12">
-        <v>1250</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B37" s="12">
-        <v>16022017</v>
+        <v>7032017</v>
       </c>
       <c r="C37" s="22">
-        <v>0.36930000000000002</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="D37" s="12">
-        <v>1344</v>
+        <v>1108</v>
       </c>
       <c r="E37" s="12">
-        <v>1250</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B38" s="12">
-        <v>16022017</v>
+        <v>7032017</v>
       </c>
       <c r="C38" s="22">
-        <v>0.36630000000000001</v>
+        <v>0.67979999999999996</v>
       </c>
       <c r="D38" s="12">
-        <v>1344</v>
+        <v>1108</v>
       </c>
       <c r="E38" s="12">
-        <v>1250</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B39" s="12">
-        <v>16022017</v>
+        <v>15022017</v>
       </c>
       <c r="C39" s="22">
-        <v>0.56820000000000004</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="D39" s="12">
-        <v>1250</v>
+        <v>1023</v>
       </c>
       <c r="E39" s="12">
-        <v>1250</v>
+        <v>929</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B40" s="12">
         <v>16022017</v>
       </c>
       <c r="C40" s="22">
-        <v>0.55179999999999996</v>
+        <v>0.51729999999999998</v>
       </c>
       <c r="D40" s="12">
-        <v>1250</v>
+        <v>1331</v>
       </c>
       <c r="E40" s="12">
         <v>1250</v>
@@ -18393,118 +18402,118 @@
     </row>
     <row r="41" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B41" s="12">
-        <v>16022017</v>
+        <v>17022017</v>
       </c>
       <c r="C41" s="22">
-        <v>0.54890000000000005</v>
+        <v>0.57750000000000001</v>
       </c>
       <c r="D41" s="12">
-        <v>1250</v>
+        <v>937</v>
       </c>
       <c r="E41" s="12">
-        <v>1250</v>
+        <v>854</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B42" s="12">
-        <v>16022017</v>
+        <v>18022017</v>
       </c>
       <c r="C42" s="22">
-        <v>0.49030000000000001</v>
+        <v>0.68289999999999995</v>
       </c>
       <c r="D42" s="12">
-        <v>1257</v>
+        <v>1650</v>
       </c>
       <c r="E42" s="12">
-        <v>1250</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B43" s="12">
-        <v>16022017</v>
+        <v>19022017</v>
       </c>
       <c r="C43" s="22">
-        <v>0.47660000000000002</v>
+        <v>0.72170000000000001</v>
       </c>
       <c r="D43" s="12">
-        <v>1257</v>
+        <v>1638</v>
       </c>
       <c r="E43" s="12">
-        <v>1250</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B44" s="12">
-        <v>16022017</v>
+        <v>20022017</v>
       </c>
       <c r="C44" s="22">
-        <v>0.49159999999999998</v>
+        <v>0.71160000000000001</v>
       </c>
       <c r="D44" s="12">
-        <v>1257</v>
+        <v>1126</v>
       </c>
       <c r="E44" s="12">
-        <v>1250</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B45" s="12">
-        <v>16022017</v>
+        <v>7032017</v>
       </c>
       <c r="C45" s="22">
-        <v>0.5645</v>
+        <v>0.59819999999999995</v>
       </c>
       <c r="D45" s="12">
-        <v>1303</v>
+        <v>1112</v>
       </c>
       <c r="E45" s="12">
-        <v>1250</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B46" s="12">
-        <v>16022017</v>
+        <v>15022017</v>
       </c>
       <c r="C46" s="22">
-        <v>0.55530000000000002</v>
+        <v>0.26229999999999998</v>
       </c>
       <c r="D46" s="12">
-        <v>1303</v>
+        <v>1029</v>
       </c>
       <c r="E46" s="12">
-        <v>1250</v>
+        <v>929</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B47" s="12">
         <v>16022017</v>
       </c>
       <c r="C47" s="22">
-        <v>0.56499999999999995</v>
+        <v>0.45729999999999998</v>
       </c>
       <c r="D47" s="12">
-        <v>1303</v>
+        <v>1336</v>
       </c>
       <c r="E47" s="12">
         <v>1250</v>
@@ -18512,118 +18521,118 @@
     </row>
     <row r="48" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B48" s="12">
-        <v>16022017</v>
+        <v>17022017</v>
       </c>
       <c r="C48" s="22">
-        <v>0.56079999999999997</v>
+        <v>0.438</v>
       </c>
       <c r="D48" s="12">
-        <v>1309</v>
+        <v>943</v>
       </c>
       <c r="E48" s="12">
-        <v>1250</v>
+        <v>854</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B49" s="12">
-        <v>16022017</v>
+        <v>18022017</v>
       </c>
       <c r="C49" s="22">
-        <v>0.53769999999999996</v>
+        <v>0.4894</v>
       </c>
       <c r="D49" s="12">
-        <v>1309</v>
+        <v>1656</v>
       </c>
       <c r="E49" s="12">
-        <v>1250</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B50" s="12">
-        <v>16022017</v>
+        <v>19022017</v>
       </c>
       <c r="C50" s="22">
-        <v>0.55210000000000004</v>
+        <v>0.54339999999999999</v>
       </c>
       <c r="D50" s="12">
-        <v>1309</v>
+        <v>1643</v>
       </c>
       <c r="E50" s="12">
-        <v>1250</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B51" s="12">
-        <v>16022017</v>
+        <v>20022017</v>
       </c>
       <c r="C51" s="22">
-        <v>0.56930000000000003</v>
+        <v>0.55310000000000004</v>
       </c>
       <c r="D51" s="12">
-        <v>1314</v>
+        <v>1131</v>
       </c>
       <c r="E51" s="12">
-        <v>1250</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B52" s="12">
-        <v>16022017</v>
+        <v>7032017</v>
       </c>
       <c r="C52" s="22">
-        <v>0.5595</v>
+        <v>0.72170000000000001</v>
       </c>
       <c r="D52" s="12">
-        <v>1314</v>
+        <v>1034</v>
       </c>
       <c r="E52" s="12">
-        <v>1250</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B53" s="12">
-        <v>16022017</v>
+        <v>15022017</v>
       </c>
       <c r="C53" s="22">
-        <v>0.56059999999999999</v>
+        <v>0.45279999999999998</v>
       </c>
       <c r="D53" s="12">
-        <v>1314</v>
+        <v>935</v>
       </c>
       <c r="E53" s="12">
-        <v>1250</v>
+        <v>929</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B54" s="12">
         <v>16022017</v>
       </c>
       <c r="C54" s="22">
-        <v>0.55789999999999995</v>
+        <v>0.56820000000000004</v>
       </c>
       <c r="D54" s="12">
-        <v>1320</v>
+        <v>1250</v>
       </c>
       <c r="E54" s="12">
         <v>1250</v>
@@ -18631,118 +18640,118 @@
     </row>
     <row r="55" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B55" s="12">
-        <v>16022017</v>
+        <v>17022017</v>
       </c>
       <c r="C55" s="22">
-        <v>0.51429999999999998</v>
+        <v>0.59370000000000001</v>
       </c>
       <c r="D55" s="12">
-        <v>1320</v>
+        <v>858</v>
       </c>
       <c r="E55" s="12">
-        <v>1250</v>
+        <v>854</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B56" s="12">
-        <v>16022017</v>
+        <v>18022017</v>
       </c>
       <c r="C56" s="22">
-        <v>0.54679999999999995</v>
+        <v>0.68459999999999999</v>
       </c>
       <c r="D56" s="12">
-        <v>1320</v>
+        <v>1608</v>
       </c>
       <c r="E56" s="12">
-        <v>1250</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B57" s="12">
-        <v>16022017</v>
+        <v>19022017</v>
       </c>
       <c r="C57" s="22">
-        <v>0.54430000000000001</v>
+        <v>0.71860000000000002</v>
       </c>
       <c r="D57" s="12">
-        <v>1325</v>
+        <v>1559</v>
       </c>
       <c r="E57" s="12">
-        <v>1250</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B58" s="12">
-        <v>16022017</v>
+        <v>20022017</v>
       </c>
       <c r="C58" s="22">
-        <v>0.54830000000000001</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="D58" s="12">
-        <v>1325</v>
+        <v>1052</v>
       </c>
       <c r="E58" s="12">
-        <v>1250</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B59" s="12">
-        <v>16022017</v>
+        <v>7032017</v>
       </c>
       <c r="C59" s="22">
-        <v>0.55769999999999997</v>
+        <v>0.69979999999999998</v>
       </c>
       <c r="D59" s="12">
-        <v>1325</v>
+        <v>1034</v>
       </c>
       <c r="E59" s="12">
-        <v>1250</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B60" s="12">
-        <v>16022017</v>
+        <v>15022017</v>
       </c>
       <c r="C60" s="22">
-        <v>0.51839999999999997</v>
+        <v>0.46810000000000002</v>
       </c>
       <c r="D60" s="12">
-        <v>1331</v>
+        <v>935</v>
       </c>
       <c r="E60" s="12">
-        <v>1250</v>
+        <v>929</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B61" s="12">
         <v>16022017</v>
       </c>
       <c r="C61" s="22">
-        <v>0.51859999999999995</v>
+        <v>0.55179999999999996</v>
       </c>
       <c r="D61" s="12">
-        <v>1331</v>
+        <v>1250</v>
       </c>
       <c r="E61" s="12">
         <v>1250</v>
@@ -18750,132 +18759,132 @@
     </row>
     <row r="62" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B62" s="12">
-        <v>16022017</v>
+        <v>17022017</v>
       </c>
       <c r="C62" s="22">
-        <v>0.51729999999999998</v>
+        <v>0.57189999999999996</v>
       </c>
       <c r="D62" s="12">
-        <v>1331</v>
+        <v>858</v>
       </c>
       <c r="E62" s="12">
-        <v>1250</v>
+        <v>854</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="B63" s="12">
-        <v>16022017</v>
+        <v>18022017</v>
       </c>
       <c r="C63" s="22">
-        <v>0.45729999999999998</v>
+        <v>0.66839999999999999</v>
       </c>
       <c r="D63" s="12">
-        <v>1336</v>
+        <v>1608</v>
       </c>
       <c r="E63" s="12">
-        <v>1250</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B64" s="12">
-        <v>16022017</v>
+        <v>19022017</v>
       </c>
       <c r="C64" s="22">
-        <v>0.45729999999999998</v>
+        <v>0.71309999999999996</v>
       </c>
       <c r="D64" s="12">
-        <v>1336</v>
+        <v>1559</v>
       </c>
       <c r="E64" s="12">
-        <v>1250</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B65" s="12">
-        <v>16022017</v>
+        <v>20022017</v>
       </c>
       <c r="C65" s="22">
-        <v>0.36209999999999998</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="D65" s="12">
-        <v>1336</v>
+        <v>1052</v>
       </c>
       <c r="E65" s="12">
-        <v>1250</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B66" s="12">
-        <v>17022017</v>
+        <v>7032017</v>
       </c>
       <c r="C66" s="22">
-        <v>0.42380000000000001</v>
+        <v>0.70340000000000003</v>
       </c>
       <c r="D66" s="12">
-        <v>854</v>
+        <v>1034</v>
       </c>
       <c r="E66" s="12">
-        <v>854</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B67" s="12">
-        <v>17022017</v>
+        <v>15022017</v>
       </c>
       <c r="C67" s="22">
-        <v>0.4345</v>
+        <v>0.46810000000000002</v>
       </c>
       <c r="D67" s="12">
-        <v>854</v>
+        <v>935</v>
       </c>
       <c r="E67" s="12">
-        <v>854</v>
+        <v>929</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B68" s="12">
-        <v>17022017</v>
+        <v>16022017</v>
       </c>
       <c r="C68" s="22">
-        <v>0.43990000000000001</v>
+        <v>0.54890000000000005</v>
       </c>
       <c r="D68" s="12">
-        <v>854</v>
+        <v>1250</v>
       </c>
       <c r="E68" s="12">
-        <v>854</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B69" s="12">
         <v>17022017</v>
       </c>
       <c r="C69" s="22">
-        <v>0.59370000000000001</v>
+        <v>0.5917</v>
       </c>
       <c r="D69" s="12">
         <v>858</v>
@@ -18886,19 +18895,19 @@
     </row>
     <row r="70" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B70" s="12">
-        <v>17022017</v>
+        <v>18022017</v>
       </c>
       <c r="C70" s="22">
-        <v>0.57189999999999996</v>
+        <v>0.68069999999999997</v>
       </c>
       <c r="D70" s="12">
-        <v>858</v>
+        <v>1608</v>
       </c>
       <c r="E70" s="12">
-        <v>854</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -18906,98 +18915,98 @@
         <v>19</v>
       </c>
       <c r="B71" s="12">
-        <v>17022017</v>
+        <v>19022017</v>
       </c>
       <c r="C71" s="22">
-        <v>0.5917</v>
+        <v>0.7167</v>
       </c>
       <c r="D71" s="12">
-        <v>858</v>
+        <v>1559</v>
       </c>
       <c r="E71" s="12">
-        <v>854</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B72" s="12">
-        <v>17022017</v>
+        <v>20022017</v>
       </c>
       <c r="C72" s="22">
-        <v>0.51680000000000004</v>
+        <v>0.72709999999999997</v>
       </c>
       <c r="D72" s="12">
-        <v>904</v>
+        <v>1052</v>
       </c>
       <c r="E72" s="12">
-        <v>854</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B73" s="12">
-        <v>17022017</v>
+        <v>7032017</v>
       </c>
       <c r="C73" s="22">
-        <v>0.50919999999999999</v>
+        <v>0.59819999999999995</v>
       </c>
       <c r="D73" s="12">
-        <v>904</v>
+        <v>1112</v>
       </c>
       <c r="E73" s="12">
-        <v>854</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B74" s="12">
-        <v>17022017</v>
+        <v>15022017</v>
       </c>
       <c r="C74" s="22">
-        <v>0.53029999999999999</v>
+        <v>0.251</v>
       </c>
       <c r="D74" s="12">
-        <v>904</v>
+        <v>1029</v>
       </c>
       <c r="E74" s="12">
-        <v>854</v>
+        <v>929</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B75" s="12">
-        <v>17022017</v>
+        <v>16022017</v>
       </c>
       <c r="C75" s="22">
-        <v>0.59079999999999999</v>
+        <v>0.45729999999999998</v>
       </c>
       <c r="D75" s="12">
-        <v>909</v>
+        <v>1336</v>
       </c>
       <c r="E75" s="12">
-        <v>854</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B76" s="12">
         <v>17022017</v>
       </c>
       <c r="C76" s="22">
-        <v>0.60229999999999995</v>
+        <v>0.44879999999999998</v>
       </c>
       <c r="D76" s="12">
-        <v>909</v>
+        <v>943</v>
       </c>
       <c r="E76" s="12">
         <v>854</v>
@@ -19005,118 +19014,118 @@
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B77" s="12">
-        <v>17022017</v>
+        <v>18022017</v>
       </c>
       <c r="C77" s="22">
-        <v>0.58679999999999999</v>
+        <v>0.47720000000000001</v>
       </c>
       <c r="D77" s="12">
-        <v>909</v>
+        <v>1656</v>
       </c>
       <c r="E77" s="12">
-        <v>854</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B78" s="12">
-        <v>17022017</v>
+        <v>19022017</v>
       </c>
       <c r="C78" s="22">
-        <v>0.60040000000000004</v>
+        <v>0.52890000000000004</v>
       </c>
       <c r="D78" s="12">
-        <v>915</v>
+        <v>1643</v>
       </c>
       <c r="E78" s="12">
-        <v>854</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B79" s="12">
-        <v>17022017</v>
+        <v>20022017</v>
       </c>
       <c r="C79" s="22">
-        <v>0.59050000000000002</v>
+        <v>0.54469999999999996</v>
       </c>
       <c r="D79" s="12">
-        <v>915</v>
+        <v>1131</v>
       </c>
       <c r="E79" s="12">
-        <v>854</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B80" s="12">
-        <v>17022017</v>
+        <v>7032017</v>
       </c>
       <c r="C80" s="22">
-        <v>0.59709999999999996</v>
+        <v>0.70489999999999997</v>
       </c>
       <c r="D80" s="12">
-        <v>915</v>
+        <v>1038</v>
       </c>
       <c r="E80" s="12">
-        <v>854</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B81" s="12">
-        <v>17022017</v>
+        <v>15022017</v>
       </c>
       <c r="C81" s="22">
-        <v>0.60299999999999998</v>
+        <v>0.48920000000000002</v>
       </c>
       <c r="D81" s="12">
-        <v>920</v>
+        <v>941</v>
       </c>
       <c r="E81" s="12">
-        <v>854</v>
+        <v>929</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B82" s="12">
-        <v>17022017</v>
+        <v>16022017</v>
       </c>
       <c r="C82" s="22">
-        <v>0.60050000000000003</v>
+        <v>0.49030000000000001</v>
       </c>
       <c r="D82" s="12">
-        <v>920</v>
+        <v>1257</v>
       </c>
       <c r="E82" s="12">
-        <v>854</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B83" s="12">
         <v>17022017</v>
       </c>
       <c r="C83" s="22">
-        <v>0.60070000000000001</v>
+        <v>0.51680000000000004</v>
       </c>
       <c r="D83" s="12">
-        <v>920</v>
+        <v>904</v>
       </c>
       <c r="E83" s="12">
         <v>854</v>
@@ -19124,118 +19133,118 @@
     </row>
     <row r="84" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B84" s="12">
-        <v>17022017</v>
+        <v>18022017</v>
       </c>
       <c r="C84" s="22">
-        <v>0.60109999999999997</v>
+        <v>0.63339999999999996</v>
       </c>
       <c r="D84" s="12">
-        <v>926</v>
+        <v>1613</v>
       </c>
       <c r="E84" s="12">
-        <v>854</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B85" s="12">
-        <v>17022017</v>
+        <v>19022017</v>
       </c>
       <c r="C85" s="22">
-        <v>0.58289999999999997</v>
+        <v>0.68889999999999996</v>
       </c>
       <c r="D85" s="12">
-        <v>926</v>
+        <v>1607</v>
       </c>
       <c r="E85" s="12">
-        <v>854</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B86" s="12">
-        <v>17022017</v>
+        <v>20022017</v>
       </c>
       <c r="C86" s="22">
-        <v>0.56200000000000006</v>
+        <v>0.70979999999999999</v>
       </c>
       <c r="D86" s="12">
-        <v>926</v>
+        <v>1057</v>
       </c>
       <c r="E86" s="12">
-        <v>854</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B87" s="12">
-        <v>17022017</v>
+        <v>7032017</v>
       </c>
       <c r="C87" s="22">
-        <v>0.58289999999999997</v>
+        <v>0.71709999999999996</v>
       </c>
       <c r="D87" s="12">
-        <v>932</v>
+        <v>1038</v>
       </c>
       <c r="E87" s="12">
-        <v>854</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B88" s="12">
-        <v>17022017</v>
+        <v>15022017</v>
       </c>
       <c r="C88" s="22">
-        <v>0.58289999999999997</v>
+        <v>0.47639999999999999</v>
       </c>
       <c r="D88" s="12">
-        <v>932</v>
+        <v>941</v>
       </c>
       <c r="E88" s="12">
-        <v>854</v>
+        <v>929</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B89" s="12">
-        <v>17022017</v>
+        <v>16022017</v>
       </c>
       <c r="C89" s="22">
-        <v>0.60589999999999999</v>
+        <v>0.47660000000000002</v>
       </c>
       <c r="D89" s="12">
-        <v>932</v>
+        <v>1257</v>
       </c>
       <c r="E89" s="12">
-        <v>854</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B90" s="12">
         <v>17022017</v>
       </c>
       <c r="C90" s="22">
-        <v>0.5786</v>
+        <v>0.50919999999999999</v>
       </c>
       <c r="D90" s="12">
-        <v>937</v>
+        <v>904</v>
       </c>
       <c r="E90" s="12">
         <v>854</v>
@@ -19243,118 +19252,118 @@
     </row>
     <row r="91" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B91" s="12">
-        <v>17022017</v>
+        <v>18022017</v>
       </c>
       <c r="C91" s="22">
-        <v>0.57920000000000005</v>
+        <v>0.6179</v>
       </c>
       <c r="D91" s="12">
-        <v>937</v>
+        <v>1613</v>
       </c>
       <c r="E91" s="12">
-        <v>854</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B92" s="12">
-        <v>17022017</v>
+        <v>19022017</v>
       </c>
       <c r="C92" s="22">
-        <v>0.57750000000000001</v>
+        <v>0.67620000000000002</v>
       </c>
       <c r="D92" s="12">
-        <v>937</v>
+        <v>1607</v>
       </c>
       <c r="E92" s="12">
-        <v>854</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B93" s="12">
-        <v>17022017</v>
+        <v>20022017</v>
       </c>
       <c r="C93" s="22">
-        <v>0.438</v>
+        <v>0.70979999999999999</v>
       </c>
       <c r="D93" s="12">
-        <v>943</v>
+        <v>1057</v>
       </c>
       <c r="E93" s="12">
-        <v>854</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="B94" s="12">
-        <v>17022017</v>
+        <v>7032017</v>
       </c>
       <c r="C94" s="22">
-        <v>0.44879999999999998</v>
+        <v>0.71289999999999998</v>
       </c>
       <c r="D94" s="12">
-        <v>943</v>
+        <v>1038</v>
       </c>
       <c r="E94" s="12">
-        <v>854</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B95" s="12">
-        <v>17022017</v>
+        <v>15022017</v>
       </c>
       <c r="C95" s="22">
-        <v>0.44879999999999998</v>
+        <v>0.48559999999999998</v>
       </c>
       <c r="D95" s="12">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E95" s="12">
-        <v>854</v>
+        <v>929</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B96" s="12">
-        <v>17022017</v>
+        <v>16022017</v>
       </c>
       <c r="C96" s="22">
-        <v>0.70669999999999999</v>
+        <v>0.49159999999999998</v>
       </c>
       <c r="D96" s="12">
-        <v>951</v>
+        <v>1257</v>
       </c>
       <c r="E96" s="12">
-        <v>854</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B97" s="12">
         <v>17022017</v>
       </c>
       <c r="C97" s="22">
-        <v>0.71120000000000005</v>
+        <v>0.53029999999999999</v>
       </c>
       <c r="D97" s="12">
-        <v>951</v>
+        <v>904</v>
       </c>
       <c r="E97" s="12">
         <v>854</v>
@@ -19362,135 +19371,135 @@
     </row>
     <row r="98" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B98" s="12">
-        <v>17022017</v>
+        <v>18022017</v>
       </c>
       <c r="C98" s="22">
-        <v>0.71540000000000004</v>
+        <v>0.63870000000000005</v>
       </c>
       <c r="D98" s="12">
-        <v>951</v>
+        <v>1613</v>
       </c>
       <c r="E98" s="12">
-        <v>854</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B99" s="12">
-        <v>18022017</v>
+        <v>19022017</v>
       </c>
       <c r="C99" s="22">
-        <v>0.53369999999999995</v>
+        <v>0.6865</v>
       </c>
       <c r="D99" s="12">
-        <v>1706</v>
+        <v>1607</v>
       </c>
       <c r="E99" s="12">
-        <v>1608</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B100" s="12">
-        <v>18022017</v>
+        <v>20022017</v>
       </c>
       <c r="C100" s="22">
-        <v>0.4844</v>
+        <v>0.70709999999999995</v>
       </c>
       <c r="D100" s="12">
-        <v>1706</v>
+        <v>1057</v>
       </c>
       <c r="E100" s="12">
-        <v>1608</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B101" s="12">
-        <v>18022017</v>
+        <v>7032017</v>
       </c>
       <c r="C101" s="22">
-        <v>0.4844</v>
+        <v>0.59819999999999995</v>
       </c>
       <c r="D101" s="12">
-        <v>1706</v>
+        <v>1112</v>
       </c>
       <c r="E101" s="12">
-        <v>1608</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B102" s="12">
-        <v>18022017</v>
+        <v>15022017</v>
       </c>
       <c r="C102" s="22">
-        <v>0.68459999999999999</v>
+        <v>0.2432</v>
       </c>
       <c r="D102" s="12">
-        <v>1608</v>
+        <v>1029</v>
       </c>
       <c r="E102" s="12">
-        <v>1608</v>
+        <v>929</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B103" s="12">
-        <v>18022017</v>
+        <v>16022017</v>
       </c>
       <c r="C103" s="22">
-        <v>0.66839999999999999</v>
+        <v>0.36209999999999998</v>
       </c>
       <c r="D103" s="12">
-        <v>1608</v>
+        <v>1336</v>
       </c>
       <c r="E103" s="12">
-        <v>1608</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B104" s="12">
-        <v>18022017</v>
+        <v>17022017</v>
       </c>
       <c r="C104" s="22">
-        <v>0.68069999999999997</v>
+        <v>0.44879999999999998</v>
       </c>
       <c r="D104" s="12">
-        <v>1608</v>
+        <v>943</v>
       </c>
       <c r="E104" s="12">
-        <v>1608</v>
+        <v>854</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B105" s="12">
         <v>18022017</v>
       </c>
       <c r="C105" s="22">
-        <v>0.63339999999999996</v>
+        <v>0.4803</v>
       </c>
       <c r="D105" s="12">
-        <v>1613</v>
+        <v>1656</v>
       </c>
       <c r="E105" s="12">
         <v>1608</v>
@@ -19498,36 +19507,36 @@
     </row>
     <row r="106" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B106" s="12">
-        <v>18022017</v>
+        <v>19022017</v>
       </c>
       <c r="C106" s="22">
-        <v>0.6179</v>
+        <v>0.5282</v>
       </c>
       <c r="D106" s="12">
-        <v>1613</v>
+        <v>1643</v>
       </c>
       <c r="E106" s="12">
-        <v>1608</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B107" s="12">
-        <v>18022017</v>
+        <v>20022017</v>
       </c>
       <c r="C107" s="22">
-        <v>0.63870000000000005</v>
+        <v>0.54649999999999999</v>
       </c>
       <c r="D107" s="12">
-        <v>1613</v>
+        <v>1131</v>
       </c>
       <c r="E107" s="12">
-        <v>1608</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -19535,81 +19544,81 @@
         <v>24</v>
       </c>
       <c r="B108" s="12">
-        <v>18022017</v>
+        <v>7032017</v>
       </c>
       <c r="C108" s="22">
-        <v>0.68089999999999995</v>
+        <v>0.67390000000000005</v>
       </c>
       <c r="D108" s="12">
-        <v>1619</v>
+        <v>1042</v>
       </c>
       <c r="E108" s="12">
-        <v>1608</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="109" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B109" s="12">
-        <v>18022017</v>
+        <v>15022017</v>
       </c>
       <c r="C109" s="22">
-        <v>0.70350000000000001</v>
+        <v>0.39479999999999998</v>
       </c>
       <c r="D109" s="12">
-        <v>1619</v>
+        <v>949</v>
       </c>
       <c r="E109" s="12">
-        <v>1608</v>
+        <v>929</v>
       </c>
     </row>
     <row r="110" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B110" s="12">
-        <v>18022017</v>
+        <v>16022017</v>
       </c>
       <c r="C110" s="22">
-        <v>0.68610000000000004</v>
+        <v>0.5645</v>
       </c>
       <c r="D110" s="12">
-        <v>1619</v>
+        <v>1303</v>
       </c>
       <c r="E110" s="12">
-        <v>1608</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B111" s="12">
-        <v>18022017</v>
+        <v>17022017</v>
       </c>
       <c r="C111" s="22">
-        <v>0.66800000000000004</v>
+        <v>0.59079999999999999</v>
       </c>
       <c r="D111" s="12">
-        <v>1625</v>
+        <v>909</v>
       </c>
       <c r="E111" s="12">
-        <v>1608</v>
+        <v>854</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B112" s="12">
         <v>18022017</v>
       </c>
       <c r="C112" s="22">
-        <v>0.6804</v>
+        <v>0.68089999999999995</v>
       </c>
       <c r="D112" s="12">
-        <v>1625</v>
+        <v>1619</v>
       </c>
       <c r="E112" s="12">
         <v>1608</v>
@@ -19617,118 +19626,118 @@
     </row>
     <row r="113" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B113" s="12">
-        <v>18022017</v>
+        <v>19022017</v>
       </c>
       <c r="C113" s="22">
-        <v>0.68710000000000004</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="D113" s="12">
-        <v>1625</v>
+        <v>1613</v>
       </c>
       <c r="E113" s="12">
-        <v>1608</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B114" s="12">
-        <v>18022017</v>
+        <v>20022017</v>
       </c>
       <c r="C114" s="22">
-        <v>0.68569999999999998</v>
+        <v>0.73750000000000004</v>
       </c>
       <c r="D114" s="12">
-        <v>1631</v>
+        <v>1102</v>
       </c>
       <c r="E114" s="12">
-        <v>1608</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="115" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B115" s="12">
-        <v>18022017</v>
+        <v>7032017</v>
       </c>
       <c r="C115" s="22">
-        <v>0.68530000000000002</v>
+        <v>0.67159999999999997</v>
       </c>
       <c r="D115" s="12">
-        <v>1631</v>
+        <v>1042</v>
       </c>
       <c r="E115" s="12">
-        <v>1608</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B116" s="12">
-        <v>18022017</v>
+        <v>15022017</v>
       </c>
       <c r="C116" s="22">
-        <v>0.66659999999999997</v>
+        <v>0.48620000000000002</v>
       </c>
       <c r="D116" s="12">
-        <v>1631</v>
+        <v>949</v>
       </c>
       <c r="E116" s="12">
-        <v>1608</v>
+        <v>929</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B117" s="12">
-        <v>18022017</v>
+        <v>16022017</v>
       </c>
       <c r="C117" s="22">
-        <v>0.66590000000000005</v>
+        <v>0.55530000000000002</v>
       </c>
       <c r="D117" s="12">
-        <v>1637</v>
+        <v>1303</v>
       </c>
       <c r="E117" s="12">
-        <v>1608</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="118" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B118" s="12">
-        <v>18022017</v>
+        <v>17022017</v>
       </c>
       <c r="C118" s="22">
-        <v>0.66159999999999997</v>
+        <v>0.60229999999999995</v>
       </c>
       <c r="D118" s="12">
-        <v>1637</v>
+        <v>909</v>
       </c>
       <c r="E118" s="12">
-        <v>1608</v>
+        <v>854</v>
       </c>
     </row>
     <row r="119" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B119" s="12">
         <v>18022017</v>
       </c>
       <c r="C119" s="22">
-        <v>0.66569999999999996</v>
+        <v>0.70350000000000001</v>
       </c>
       <c r="D119" s="12">
-        <v>1637</v>
+        <v>1619</v>
       </c>
       <c r="E119" s="12">
         <v>1608</v>
@@ -19736,118 +19745,118 @@
     </row>
     <row r="120" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B120" s="12">
-        <v>18022017</v>
+        <v>19022017</v>
       </c>
       <c r="C120" s="22">
-        <v>0.68540000000000001</v>
+        <v>0.70860000000000001</v>
       </c>
       <c r="D120" s="12">
-        <v>1644</v>
+        <v>1613</v>
       </c>
       <c r="E120" s="12">
-        <v>1608</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="121" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B121" s="12">
-        <v>18022017</v>
+        <v>20022017</v>
       </c>
       <c r="C121" s="22">
-        <v>0.68969999999999998</v>
+        <v>0.73109999999999997</v>
       </c>
       <c r="D121" s="12">
-        <v>1644</v>
+        <v>1102</v>
       </c>
       <c r="E121" s="12">
-        <v>1608</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B122" s="12">
-        <v>18022017</v>
+        <v>7032017</v>
       </c>
       <c r="C122" s="22">
-        <v>0.69899999999999995</v>
+        <v>0.68879999999999997</v>
       </c>
       <c r="D122" s="12">
-        <v>1644</v>
+        <v>1042</v>
       </c>
       <c r="E122" s="12">
-        <v>1608</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="123" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B123" s="12">
-        <v>18022017</v>
+        <v>15022017</v>
       </c>
       <c r="C123" s="22">
-        <v>0.68379999999999996</v>
+        <v>0.43290000000000001</v>
       </c>
       <c r="D123" s="12">
-        <v>1650</v>
+        <v>949</v>
       </c>
       <c r="E123" s="12">
-        <v>1608</v>
+        <v>929</v>
       </c>
     </row>
     <row r="124" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B124" s="12">
-        <v>18022017</v>
+        <v>16022017</v>
       </c>
       <c r="C124" s="22">
-        <v>0.68289999999999995</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="D124" s="12">
-        <v>1650</v>
+        <v>1303</v>
       </c>
       <c r="E124" s="12">
-        <v>1608</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="125" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B125" s="12">
-        <v>18022017</v>
+        <v>17022017</v>
       </c>
       <c r="C125" s="22">
-        <v>0.68289999999999995</v>
+        <v>0.58679999999999999</v>
       </c>
       <c r="D125" s="12">
-        <v>1650</v>
+        <v>909</v>
       </c>
       <c r="E125" s="12">
-        <v>1608</v>
+        <v>854</v>
       </c>
     </row>
     <row r="126" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B126" s="12">
         <v>18022017</v>
       </c>
       <c r="C126" s="22">
-        <v>0.4894</v>
+        <v>0.68610000000000004</v>
       </c>
       <c r="D126" s="12">
-        <v>1656</v>
+        <v>1619</v>
       </c>
       <c r="E126" s="12">
         <v>1608</v>
@@ -19855,135 +19864,135 @@
     </row>
     <row r="127" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B127" s="12">
-        <v>18022017</v>
+        <v>19022017</v>
       </c>
       <c r="C127" s="22">
-        <v>0.47720000000000001</v>
+        <v>0.7228</v>
       </c>
       <c r="D127" s="12">
-        <v>1656</v>
+        <v>1613</v>
       </c>
       <c r="E127" s="12">
-        <v>1608</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="128" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B128" s="12">
-        <v>18022017</v>
+        <v>20022017</v>
       </c>
       <c r="C128" s="22">
-        <v>0.4803</v>
+        <v>0.73980000000000001</v>
       </c>
       <c r="D128" s="12">
-        <v>1656</v>
+        <v>1102</v>
       </c>
       <c r="E128" s="12">
-        <v>1608</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="129" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B129" s="12">
-        <v>18022017</v>
+        <v>7032017</v>
       </c>
       <c r="C129" s="22">
-        <v>0.75180000000000002</v>
+        <v>0.6724</v>
       </c>
       <c r="D129" s="12">
-        <v>1702</v>
+        <v>1047</v>
       </c>
       <c r="E129" s="12">
-        <v>1608</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B130" s="12">
-        <v>18022017</v>
+        <v>15022017</v>
       </c>
       <c r="C130" s="22">
-        <v>0.75180000000000002</v>
+        <v>0.37819999999999998</v>
       </c>
       <c r="D130" s="12">
-        <v>1702</v>
+        <v>956</v>
       </c>
       <c r="E130" s="12">
-        <v>1608</v>
+        <v>929</v>
       </c>
     </row>
     <row r="131" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B131" s="12">
-        <v>18022017</v>
+        <v>16022017</v>
       </c>
       <c r="C131" s="22">
-        <v>0.76080000000000003</v>
+        <v>0.56079999999999997</v>
       </c>
       <c r="D131" s="12">
-        <v>1702</v>
+        <v>1309</v>
       </c>
       <c r="E131" s="12">
-        <v>1608</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B132" s="12">
-        <v>19022017</v>
+        <v>17022017</v>
       </c>
       <c r="C132" s="22">
-        <v>0.71860000000000002</v>
+        <v>0.60040000000000004</v>
       </c>
       <c r="D132" s="12">
-        <v>1559</v>
+        <v>915</v>
       </c>
       <c r="E132" s="12">
-        <v>1559</v>
+        <v>854</v>
       </c>
     </row>
     <row r="133" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B133" s="12">
-        <v>19022017</v>
+        <v>18022017</v>
       </c>
       <c r="C133" s="22">
-        <v>0.71309999999999996</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="D133" s="12">
-        <v>1559</v>
+        <v>1625</v>
       </c>
       <c r="E133" s="12">
-        <v>1559</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B134" s="12">
         <v>19022017</v>
       </c>
       <c r="C134" s="22">
-        <v>0.7167</v>
+        <v>0.70309999999999995</v>
       </c>
       <c r="D134" s="12">
-        <v>1559</v>
+        <v>1619</v>
       </c>
       <c r="E134" s="12">
         <v>1559</v>
@@ -19991,115 +20000,115 @@
     </row>
     <row r="135" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B135" s="12">
-        <v>19022017</v>
+        <v>20022017</v>
       </c>
       <c r="C135" s="22">
-        <v>0.68889999999999996</v>
+        <v>0.72840000000000005</v>
       </c>
       <c r="D135" s="12">
-        <v>1607</v>
+        <v>1107</v>
       </c>
       <c r="E135" s="12">
-        <v>1559</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="136" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B136" s="12">
-        <v>19022017</v>
+        <v>7032017</v>
       </c>
       <c r="C136" s="22">
-        <v>0.67620000000000002</v>
+        <v>0.67369999999999997</v>
       </c>
       <c r="D136" s="12">
-        <v>1607</v>
+        <v>1047</v>
       </c>
       <c r="E136" s="12">
-        <v>1559</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="137" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B137" s="12">
-        <v>19022017</v>
+        <v>15022017</v>
       </c>
       <c r="C137" s="22">
-        <v>0.6865</v>
+        <v>0.47149999999999997</v>
       </c>
       <c r="D137" s="12">
-        <v>1607</v>
+        <v>956</v>
       </c>
       <c r="E137" s="12">
-        <v>1559</v>
+        <v>929</v>
       </c>
     </row>
     <row r="138" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B138" s="12">
-        <v>19022017</v>
+        <v>16022017</v>
       </c>
       <c r="C138" s="22">
-        <v>0.71599999999999997</v>
+        <v>0.53769999999999996</v>
       </c>
       <c r="D138" s="12">
-        <v>1613</v>
+        <v>1309</v>
       </c>
       <c r="E138" s="12">
-        <v>1559</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="139" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B139" s="12">
-        <v>19022017</v>
+        <v>17022017</v>
       </c>
       <c r="C139" s="22">
-        <v>0.70860000000000001</v>
+        <v>0.59050000000000002</v>
       </c>
       <c r="D139" s="12">
-        <v>1613</v>
+        <v>915</v>
       </c>
       <c r="E139" s="12">
-        <v>1559</v>
+        <v>854</v>
       </c>
     </row>
     <row r="140" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B140" s="12">
-        <v>19022017</v>
+        <v>18022017</v>
       </c>
       <c r="C140" s="22">
-        <v>0.7228</v>
+        <v>0.6804</v>
       </c>
       <c r="D140" s="12">
-        <v>1613</v>
+        <v>1625</v>
       </c>
       <c r="E140" s="12">
-        <v>1559</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="141" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B141" s="12">
         <v>19022017</v>
       </c>
       <c r="C141" s="22">
-        <v>0.70309999999999995</v>
+        <v>0.70150000000000001</v>
       </c>
       <c r="D141" s="12">
         <v>1619</v>
@@ -20113,16 +20122,16 @@
         <v>30</v>
       </c>
       <c r="B142" s="12">
-        <v>19022017</v>
+        <v>20022017</v>
       </c>
       <c r="C142" s="22">
-        <v>0.70150000000000001</v>
+        <v>0.72840000000000005</v>
       </c>
       <c r="D142" s="12">
-        <v>1619</v>
+        <v>1107</v>
       </c>
       <c r="E142" s="12">
-        <v>1559</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="143" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -20130,98 +20139,98 @@
         <v>31</v>
       </c>
       <c r="B143" s="12">
-        <v>19022017</v>
+        <v>7032017</v>
       </c>
       <c r="C143" s="22">
-        <v>0.70440000000000003</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="D143" s="12">
-        <v>1619</v>
+        <v>1047</v>
       </c>
       <c r="E143" s="12">
-        <v>1559</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="144" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B144" s="12">
-        <v>19022017</v>
+        <v>15022017</v>
       </c>
       <c r="C144" s="22">
-        <v>0.70269999999999999</v>
+        <v>0.47389999999999999</v>
       </c>
       <c r="D144" s="12">
-        <v>1624</v>
+        <v>956</v>
       </c>
       <c r="E144" s="12">
-        <v>1559</v>
+        <v>929</v>
       </c>
     </row>
     <row r="145" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B145" s="12">
-        <v>19022017</v>
+        <v>16022017</v>
       </c>
       <c r="C145" s="22">
-        <v>0.69979999999999998</v>
+        <v>0.55210000000000004</v>
       </c>
       <c r="D145" s="12">
-        <v>1624</v>
+        <v>1309</v>
       </c>
       <c r="E145" s="12">
-        <v>1559</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="146" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B146" s="12">
-        <v>19022017</v>
+        <v>17022017</v>
       </c>
       <c r="C146" s="22">
-        <v>0.70040000000000002</v>
+        <v>0.59709999999999996</v>
       </c>
       <c r="D146" s="12">
-        <v>1624</v>
+        <v>915</v>
       </c>
       <c r="E146" s="12">
-        <v>1559</v>
+        <v>854</v>
       </c>
     </row>
     <row r="147" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B147" s="12">
-        <v>19022017</v>
+        <v>18022017</v>
       </c>
       <c r="C147" s="22">
-        <v>0.70950000000000002</v>
+        <v>0.68710000000000004</v>
       </c>
       <c r="D147" s="12">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="E147" s="12">
-        <v>1559</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="148" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B148" s="12">
         <v>19022017</v>
       </c>
       <c r="C148" s="22">
-        <v>0.70079999999999998</v>
+        <v>0.70440000000000003</v>
       </c>
       <c r="D148" s="12">
-        <v>1628</v>
+        <v>1619</v>
       </c>
       <c r="E148" s="12">
         <v>1559</v>
@@ -20229,118 +20238,118 @@
     </row>
     <row r="149" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B149" s="12">
-        <v>19022017</v>
+        <v>20022017</v>
       </c>
       <c r="C149" s="22">
-        <v>0.72009999999999996</v>
+        <v>0.72950000000000004</v>
       </c>
       <c r="D149" s="12">
-        <v>1628</v>
+        <v>1107</v>
       </c>
       <c r="E149" s="12">
-        <v>1559</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="150" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B150" s="12">
-        <v>19022017</v>
+        <v>7032017</v>
       </c>
       <c r="C150" s="22">
-        <v>0.72699999999999998</v>
+        <v>0.67090000000000005</v>
       </c>
       <c r="D150" s="12">
-        <v>1634</v>
+        <v>1051</v>
       </c>
       <c r="E150" s="12">
-        <v>1559</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="151" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B151" s="12">
-        <v>19022017</v>
+        <v>15022017</v>
       </c>
       <c r="C151" s="22">
-        <v>0.73329999999999995</v>
+        <v>0.37830000000000003</v>
       </c>
       <c r="D151" s="12">
-        <v>1634</v>
+        <v>1002</v>
       </c>
       <c r="E151" s="12">
-        <v>1559</v>
+        <v>929</v>
       </c>
     </row>
     <row r="152" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B152" s="12">
-        <v>19022017</v>
+        <v>16022017</v>
       </c>
       <c r="C152" s="22">
-        <v>0.73550000000000004</v>
+        <v>0.56930000000000003</v>
       </c>
       <c r="D152" s="12">
-        <v>1634</v>
+        <v>1314</v>
       </c>
       <c r="E152" s="12">
-        <v>1559</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="153" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B153" s="12">
-        <v>19022017</v>
+        <v>17022017</v>
       </c>
       <c r="C153" s="22">
-        <v>0.72470000000000001</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="D153" s="12">
-        <v>1638</v>
+        <v>920</v>
       </c>
       <c r="E153" s="12">
-        <v>1559</v>
+        <v>854</v>
       </c>
     </row>
     <row r="154" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B154" s="12">
-        <v>19022017</v>
+        <v>18022017</v>
       </c>
       <c r="C154" s="22">
-        <v>0.72470000000000001</v>
+        <v>0.68569999999999998</v>
       </c>
       <c r="D154" s="12">
-        <v>1638</v>
+        <v>1631</v>
       </c>
       <c r="E154" s="12">
-        <v>1559</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="155" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B155" s="12">
         <v>19022017</v>
       </c>
       <c r="C155" s="22">
-        <v>0.72170000000000001</v>
+        <v>0.70269999999999999</v>
       </c>
       <c r="D155" s="12">
-        <v>1638</v>
+        <v>1624</v>
       </c>
       <c r="E155" s="12">
         <v>1559</v>
@@ -20348,135 +20357,135 @@
     </row>
     <row r="156" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B156" s="12">
-        <v>19022017</v>
+        <v>20022017</v>
       </c>
       <c r="C156" s="22">
-        <v>0.54339999999999999</v>
+        <v>0.72640000000000005</v>
       </c>
       <c r="D156" s="12">
-        <v>1643</v>
+        <v>1112</v>
       </c>
       <c r="E156" s="12">
-        <v>1559</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="157" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B157" s="12">
-        <v>19022017</v>
+        <v>7032017</v>
       </c>
       <c r="C157" s="22">
-        <v>0.52890000000000004</v>
+        <v>0.69610000000000005</v>
       </c>
       <c r="D157" s="12">
-        <v>1643</v>
+        <v>1051</v>
       </c>
       <c r="E157" s="12">
-        <v>1559</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="158" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B158" s="12">
-        <v>19022017</v>
+        <v>15022017</v>
       </c>
       <c r="C158" s="22">
-        <v>0.5282</v>
+        <v>0.43480000000000002</v>
       </c>
       <c r="D158" s="12">
-        <v>1643</v>
+        <v>1002</v>
       </c>
       <c r="E158" s="12">
-        <v>1559</v>
+        <v>929</v>
       </c>
     </row>
     <row r="159" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B159" s="12">
-        <v>19022017</v>
+        <v>16022017</v>
       </c>
       <c r="C159" s="22">
-        <v>0.74319999999999997</v>
+        <v>0.5595</v>
       </c>
       <c r="D159" s="12">
-        <v>1647</v>
+        <v>1314</v>
       </c>
       <c r="E159" s="12">
-        <v>1559</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="160" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B160" s="12">
-        <v>19022017</v>
+        <v>17022017</v>
       </c>
       <c r="C160" s="22">
-        <v>0.747</v>
+        <v>0.60050000000000003</v>
       </c>
       <c r="D160" s="12">
-        <v>1647</v>
+        <v>920</v>
       </c>
       <c r="E160" s="12">
-        <v>1559</v>
+        <v>854</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B161" s="12">
-        <v>19022017</v>
+        <v>18022017</v>
       </c>
       <c r="C161" s="22">
-        <v>0.747</v>
+        <v>0.68530000000000002</v>
       </c>
       <c r="D161" s="12">
-        <v>1647</v>
+        <v>1631</v>
       </c>
       <c r="E161" s="12">
-        <v>1559</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="162" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B162" s="12">
-        <v>20022017</v>
+        <v>19022017</v>
       </c>
       <c r="C162" s="22">
-        <v>0.55700000000000005</v>
+        <v>0.69979999999999998</v>
       </c>
       <c r="D162" s="12">
-        <v>1139</v>
+        <v>1624</v>
       </c>
       <c r="E162" s="12">
-        <v>1052</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="163" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B163" s="12">
         <v>20022017</v>
       </c>
       <c r="C163" s="22">
-        <v>0.52239999999999998</v>
+        <v>0.72119999999999995</v>
       </c>
       <c r="D163" s="12">
-        <v>1139</v>
+        <v>1112</v>
       </c>
       <c r="E163" s="12">
         <v>1052</v>
@@ -20484,118 +20493,118 @@
     </row>
     <row r="164" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B164" s="12">
-        <v>20022017</v>
+        <v>7032017</v>
       </c>
       <c r="C164" s="22">
-        <v>0.52059999999999995</v>
+        <v>0.68310000000000004</v>
       </c>
       <c r="D164" s="12">
-        <v>1139</v>
+        <v>1051</v>
       </c>
       <c r="E164" s="12">
-        <v>1052</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="165" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B165" s="12">
-        <v>20022017</v>
+        <v>15022017</v>
       </c>
       <c r="C165" s="22">
-        <v>0.73399999999999999</v>
+        <v>0.33289999999999997</v>
       </c>
       <c r="D165" s="12">
-        <v>1052</v>
+        <v>1002</v>
       </c>
       <c r="E165" s="12">
-        <v>1052</v>
+        <v>929</v>
       </c>
     </row>
     <row r="166" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B166" s="12">
-        <v>20022017</v>
+        <v>16022017</v>
       </c>
       <c r="C166" s="22">
-        <v>0.71399999999999997</v>
+        <v>0.56059999999999999</v>
       </c>
       <c r="D166" s="12">
-        <v>1052</v>
+        <v>1314</v>
       </c>
       <c r="E166" s="12">
-        <v>1052</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="167" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B167" s="12">
-        <v>20022017</v>
+        <v>17022017</v>
       </c>
       <c r="C167" s="22">
-        <v>0.72709999999999997</v>
+        <v>0.60070000000000001</v>
       </c>
       <c r="D167" s="12">
-        <v>1052</v>
+        <v>920</v>
       </c>
       <c r="E167" s="12">
-        <v>1052</v>
+        <v>854</v>
       </c>
     </row>
     <row r="168" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B168" s="12">
-        <v>20022017</v>
+        <v>18022017</v>
       </c>
       <c r="C168" s="22">
-        <v>0.70979999999999999</v>
+        <v>0.66659999999999997</v>
       </c>
       <c r="D168" s="12">
-        <v>1057</v>
+        <v>1631</v>
       </c>
       <c r="E168" s="12">
-        <v>1052</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="169" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B169" s="12">
-        <v>20022017</v>
+        <v>19022017</v>
       </c>
       <c r="C169" s="22">
-        <v>0.70979999999999999</v>
+        <v>0.70040000000000002</v>
       </c>
       <c r="D169" s="12">
-        <v>1057</v>
+        <v>1624</v>
       </c>
       <c r="E169" s="12">
-        <v>1052</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="170" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B170" s="12">
         <v>20022017</v>
       </c>
       <c r="C170" s="22">
-        <v>0.70709999999999995</v>
+        <v>0.72350000000000003</v>
       </c>
       <c r="D170" s="12">
-        <v>1057</v>
+        <v>1112</v>
       </c>
       <c r="E170" s="12">
         <v>1052</v>
@@ -20603,118 +20612,118 @@
     </row>
     <row r="171" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B171" s="12">
-        <v>20022017</v>
+        <v>7032017</v>
       </c>
       <c r="C171" s="22">
-        <v>0.73750000000000004</v>
+        <v>0.69010000000000005</v>
       </c>
       <c r="D171" s="12">
-        <v>1102</v>
+        <v>1059</v>
       </c>
       <c r="E171" s="12">
-        <v>1052</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="172" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B172" s="12">
-        <v>20022017</v>
+        <v>15022017</v>
       </c>
       <c r="C172" s="22">
-        <v>0.73109999999999997</v>
+        <v>0.24840000000000001</v>
       </c>
       <c r="D172" s="12">
-        <v>1102</v>
+        <v>1009</v>
       </c>
       <c r="E172" s="12">
-        <v>1052</v>
+        <v>929</v>
       </c>
     </row>
     <row r="173" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B173" s="12">
-        <v>20022017</v>
+        <v>16022017</v>
       </c>
       <c r="C173" s="22">
-        <v>0.73980000000000001</v>
+        <v>0.55789999999999995</v>
       </c>
       <c r="D173" s="12">
-        <v>1102</v>
+        <v>1320</v>
       </c>
       <c r="E173" s="12">
-        <v>1052</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="174" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B174" s="12">
-        <v>20022017</v>
+        <v>17022017</v>
       </c>
       <c r="C174" s="22">
-        <v>0.72840000000000005</v>
+        <v>0.60109999999999997</v>
       </c>
       <c r="D174" s="12">
-        <v>1107</v>
+        <v>926</v>
       </c>
       <c r="E174" s="12">
-        <v>1052</v>
+        <v>854</v>
       </c>
     </row>
     <row r="175" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B175" s="12">
-        <v>20022017</v>
+        <v>18022017</v>
       </c>
       <c r="C175" s="22">
-        <v>0.72840000000000005</v>
+        <v>0.66590000000000005</v>
       </c>
       <c r="D175" s="12">
-        <v>1107</v>
+        <v>1637</v>
       </c>
       <c r="E175" s="12">
-        <v>1052</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="176" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B176" s="12">
-        <v>20022017</v>
+        <v>19022017</v>
       </c>
       <c r="C176" s="22">
-        <v>0.72950000000000004</v>
+        <v>0.70950000000000002</v>
       </c>
       <c r="D176" s="12">
-        <v>1107</v>
+        <v>1628</v>
       </c>
       <c r="E176" s="12">
-        <v>1052</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="177" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B177" s="12">
         <v>20022017</v>
       </c>
       <c r="C177" s="22">
-        <v>0.72640000000000005</v>
+        <v>0.73229999999999995</v>
       </c>
       <c r="D177" s="12">
-        <v>1112</v>
+        <v>1117</v>
       </c>
       <c r="E177" s="12">
         <v>1052</v>
@@ -20722,53 +20731,53 @@
     </row>
     <row r="178" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B178" s="12">
-        <v>20022017</v>
+        <v>7032017</v>
       </c>
       <c r="C178" s="22">
-        <v>0.72119999999999995</v>
+        <v>0.68079999999999996</v>
       </c>
       <c r="D178" s="12">
-        <v>1112</v>
+        <v>1059</v>
       </c>
       <c r="E178" s="12">
-        <v>1052</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="179" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B179" s="12">
-        <v>20022017</v>
+        <v>15022017</v>
       </c>
       <c r="C179" s="22">
-        <v>0.72350000000000003</v>
+        <v>0.44119999999999998</v>
       </c>
       <c r="D179" s="12">
-        <v>1112</v>
+        <v>1009</v>
       </c>
       <c r="E179" s="12">
-        <v>1052</v>
+        <v>929</v>
       </c>
     </row>
     <row r="180" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B180" s="12">
-        <v>20022017</v>
+        <v>16022017</v>
       </c>
       <c r="C180" s="22">
-        <v>0.73229999999999995</v>
+        <v>0.51429999999999998</v>
       </c>
       <c r="D180" s="12">
-        <v>1117</v>
+        <v>1320</v>
       </c>
       <c r="E180" s="12">
-        <v>1052</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="181" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -20776,64 +20785,64 @@
         <v>38</v>
       </c>
       <c r="B181" s="12">
-        <v>20022017</v>
+        <v>17022017</v>
       </c>
       <c r="C181" s="22">
-        <v>0.73080000000000001</v>
+        <v>0.58289999999999997</v>
       </c>
       <c r="D181" s="12">
-        <v>1117</v>
+        <v>926</v>
       </c>
       <c r="E181" s="12">
-        <v>1052</v>
+        <v>854</v>
       </c>
     </row>
     <row r="182" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B182" s="12">
-        <v>20022017</v>
+        <v>18022017</v>
       </c>
       <c r="C182" s="22">
-        <v>0.73129999999999995</v>
+        <v>0.66159999999999997</v>
       </c>
       <c r="D182" s="12">
-        <v>1117</v>
+        <v>1637</v>
       </c>
       <c r="E182" s="12">
-        <v>1052</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="183" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B183" s="12">
-        <v>20022017</v>
+        <v>19022017</v>
       </c>
       <c r="C183" s="22">
-        <v>0.72419999999999995</v>
+        <v>0.70079999999999998</v>
       </c>
       <c r="D183" s="12">
-        <v>1121</v>
+        <v>1628</v>
       </c>
       <c r="E183" s="12">
-        <v>1052</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="184" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B184" s="12">
         <v>20022017</v>
       </c>
       <c r="C184" s="22">
-        <v>0.72299999999999998</v>
+        <v>0.73080000000000001</v>
       </c>
       <c r="D184" s="12">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="E184" s="12">
         <v>1052</v>
@@ -20841,118 +20850,118 @@
     </row>
     <row r="185" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B185" s="12">
-        <v>20022017</v>
+        <v>7032017</v>
       </c>
       <c r="C185" s="22">
-        <v>0.73199999999999998</v>
+        <v>0.67769999999999997</v>
       </c>
       <c r="D185" s="12">
-        <v>1121</v>
+        <v>1059</v>
       </c>
       <c r="E185" s="12">
-        <v>1052</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="186" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B186" s="12">
-        <v>20022017</v>
+        <v>15022017</v>
       </c>
       <c r="C186" s="22">
-        <v>0.71499999999999997</v>
+        <v>0.4405</v>
       </c>
       <c r="D186" s="12">
-        <v>1126</v>
+        <v>1009</v>
       </c>
       <c r="E186" s="12">
-        <v>1052</v>
+        <v>929</v>
       </c>
     </row>
     <row r="187" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B187" s="12">
-        <v>20022017</v>
+        <v>16022017</v>
       </c>
       <c r="C187" s="22">
-        <v>0.71330000000000005</v>
+        <v>0.54679999999999995</v>
       </c>
       <c r="D187" s="12">
-        <v>1126</v>
+        <v>1320</v>
       </c>
       <c r="E187" s="12">
-        <v>1052</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="188" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B188" s="12">
-        <v>20022017</v>
+        <v>17022017</v>
       </c>
       <c r="C188" s="22">
-        <v>0.71160000000000001</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="D188" s="12">
-        <v>1126</v>
+        <v>926</v>
       </c>
       <c r="E188" s="12">
-        <v>1052</v>
+        <v>854</v>
       </c>
     </row>
     <row r="189" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B189" s="12">
-        <v>20022017</v>
+        <v>18022017</v>
       </c>
       <c r="C189" s="22">
-        <v>0.55310000000000004</v>
+        <v>0.66569999999999996</v>
       </c>
       <c r="D189" s="12">
-        <v>1131</v>
+        <v>1637</v>
       </c>
       <c r="E189" s="12">
-        <v>1052</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="190" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B190" s="12">
-        <v>20022017</v>
+        <v>19022017</v>
       </c>
       <c r="C190" s="22">
-        <v>0.54469999999999996</v>
+        <v>0.72009999999999996</v>
       </c>
       <c r="D190" s="12">
-        <v>1131</v>
+        <v>1628</v>
       </c>
       <c r="E190" s="12">
-        <v>1052</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="191" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B191" s="12">
         <v>20022017</v>
       </c>
       <c r="C191" s="22">
-        <v>0.54649999999999999</v>
+        <v>0.73129999999999995</v>
       </c>
       <c r="D191" s="12">
-        <v>1131</v>
+        <v>1117</v>
       </c>
       <c r="E191" s="12">
         <v>1052</v>
@@ -20963,115 +20972,115 @@
         <v>48</v>
       </c>
       <c r="B192" s="12">
-        <v>20022017</v>
+        <v>7032017</v>
       </c>
       <c r="C192" s="22">
-        <v>0.75049999999999994</v>
+        <v>0.73280000000000001</v>
       </c>
       <c r="D192" s="12">
-        <v>1135</v>
+        <v>1115</v>
       </c>
       <c r="E192" s="12">
-        <v>1052</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="193" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B193" s="12">
-        <v>20022017</v>
+        <v>15022017</v>
       </c>
       <c r="C193" s="22">
-        <v>0.75049999999999994</v>
+        <v>0.51629999999999998</v>
       </c>
       <c r="D193" s="12">
-        <v>1135</v>
+        <v>1034</v>
       </c>
       <c r="E193" s="12">
-        <v>1052</v>
+        <v>929</v>
       </c>
     </row>
     <row r="194" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B194" s="12">
-        <v>20022017</v>
+        <v>17022017</v>
       </c>
       <c r="C194" s="22">
-        <v>0.75049999999999994</v>
+        <v>0.70669999999999999</v>
       </c>
       <c r="D194" s="12">
-        <v>1135</v>
+        <v>951</v>
       </c>
       <c r="E194" s="12">
-        <v>1052</v>
+        <v>854</v>
       </c>
     </row>
     <row r="195" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B195" s="12">
-        <v>7032017</v>
+        <v>18022017</v>
       </c>
       <c r="C195" s="22">
-        <v>0.61229999999999996</v>
+        <v>0.75180000000000002</v>
       </c>
       <c r="D195" s="12">
-        <v>1032</v>
+        <v>1702</v>
       </c>
       <c r="E195" s="12">
-        <v>1034</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="196" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B196" s="12">
-        <v>7032017</v>
+        <v>19022017</v>
       </c>
       <c r="C196" s="22">
-        <v>0.60119999999999996</v>
+        <v>0.74319999999999997</v>
       </c>
       <c r="D196" s="12">
-        <v>1032</v>
+        <v>1647</v>
       </c>
       <c r="E196" s="12">
-        <v>1034</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="197" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B197" s="12">
-        <v>7032017</v>
+        <v>20022017</v>
       </c>
       <c r="C197" s="22">
-        <v>0.59870000000000001</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="D197" s="12">
-        <v>1032</v>
+        <v>1135</v>
       </c>
       <c r="E197" s="12">
-        <v>1034</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="198" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B198" s="12">
         <v>7032017</v>
       </c>
       <c r="C198" s="22">
-        <v>0.72170000000000001</v>
+        <v>0.73280000000000001</v>
       </c>
       <c r="D198" s="12">
-        <v>1034</v>
+        <v>1115</v>
       </c>
       <c r="E198" s="12">
         <v>1034</v>
@@ -21079,101 +21088,101 @@
     </row>
     <row r="199" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B199" s="12">
-        <v>7032017</v>
+        <v>15022017</v>
       </c>
       <c r="C199" s="22">
-        <v>0.69979999999999998</v>
+        <v>0.51759999999999995</v>
       </c>
       <c r="D199" s="12">
         <v>1034</v>
       </c>
       <c r="E199" s="12">
-        <v>1034</v>
+        <v>929</v>
       </c>
     </row>
     <row r="200" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B200" s="12">
-        <v>7032017</v>
+        <v>17022017</v>
       </c>
       <c r="C200" s="22">
-        <v>0.70340000000000003</v>
+        <v>0.71120000000000005</v>
       </c>
       <c r="D200" s="12">
-        <v>1034</v>
+        <v>951</v>
       </c>
       <c r="E200" s="12">
-        <v>1034</v>
+        <v>854</v>
       </c>
     </row>
     <row r="201" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B201" s="12">
-        <v>7032017</v>
+        <v>18022017</v>
       </c>
       <c r="C201" s="22">
-        <v>0.70489999999999997</v>
+        <v>0.75180000000000002</v>
       </c>
       <c r="D201" s="12">
-        <v>1038</v>
+        <v>1702</v>
       </c>
       <c r="E201" s="12">
-        <v>1034</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="202" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B202" s="12">
-        <v>7032017</v>
+        <v>19022017</v>
       </c>
       <c r="C202" s="22">
-        <v>0.71709999999999996</v>
+        <v>0.747</v>
       </c>
       <c r="D202" s="12">
-        <v>1038</v>
+        <v>1647</v>
       </c>
       <c r="E202" s="12">
-        <v>1034</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="203" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B203" s="12">
-        <v>7032017</v>
+        <v>20022017</v>
       </c>
       <c r="C203" s="22">
-        <v>0.71289999999999998</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="D203" s="12">
-        <v>1038</v>
+        <v>1135</v>
       </c>
       <c r="E203" s="12">
-        <v>1034</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="204" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B204" s="12">
         <v>7032017</v>
       </c>
       <c r="C204" s="22">
-        <v>0.67390000000000005</v>
+        <v>0.73280000000000001</v>
       </c>
       <c r="D204" s="12">
-        <v>1042</v>
+        <v>1115</v>
       </c>
       <c r="E204" s="12">
         <v>1034</v>
@@ -21181,101 +21190,101 @@
     </row>
     <row r="205" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B205" s="12">
-        <v>7032017</v>
+        <v>15022017</v>
       </c>
       <c r="C205" s="22">
-        <v>0.67159999999999997</v>
+        <v>0.51759999999999995</v>
       </c>
       <c r="D205" s="12">
-        <v>1042</v>
+        <v>1034</v>
       </c>
       <c r="E205" s="12">
-        <v>1034</v>
+        <v>929</v>
       </c>
     </row>
     <row r="206" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B206" s="12">
-        <v>7032017</v>
+        <v>17022017</v>
       </c>
       <c r="C206" s="22">
-        <v>0.68879999999999997</v>
+        <v>0.71540000000000004</v>
       </c>
       <c r="D206" s="12">
-        <v>1042</v>
+        <v>951</v>
       </c>
       <c r="E206" s="12">
-        <v>1034</v>
+        <v>854</v>
       </c>
     </row>
     <row r="207" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B207" s="12">
-        <v>7032017</v>
+        <v>18022017</v>
       </c>
       <c r="C207" s="22">
-        <v>0.6724</v>
+        <v>0.76080000000000003</v>
       </c>
       <c r="D207" s="12">
-        <v>1047</v>
+        <v>1702</v>
       </c>
       <c r="E207" s="12">
-        <v>1034</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="208" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B208" s="12">
-        <v>7032017</v>
+        <v>19022017</v>
       </c>
       <c r="C208" s="22">
-        <v>0.67369999999999997</v>
+        <v>0.747</v>
       </c>
       <c r="D208" s="12">
-        <v>1047</v>
+        <v>1647</v>
       </c>
       <c r="E208" s="12">
-        <v>1034</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="209" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B209" s="12">
-        <v>7032017</v>
+        <v>20022017</v>
       </c>
       <c r="C209" s="22">
-        <v>0.66200000000000003</v>
+        <v>0.75049999999999994</v>
       </c>
       <c r="D209" s="12">
-        <v>1047</v>
+        <v>1135</v>
       </c>
       <c r="E209" s="12">
-        <v>1034</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="210" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B210" s="12">
         <v>7032017</v>
       </c>
       <c r="C210" s="22">
-        <v>0.67090000000000005</v>
+        <v>0.61229999999999996</v>
       </c>
       <c r="D210" s="12">
-        <v>1051</v>
+        <v>1032</v>
       </c>
       <c r="E210" s="12">
         <v>1034</v>
@@ -21283,101 +21292,101 @@
     </row>
     <row r="211" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B211" s="12">
-        <v>7032017</v>
+        <v>15022017</v>
       </c>
       <c r="C211" s="22">
-        <v>0.69610000000000005</v>
+        <v>0.24390000000000001</v>
       </c>
       <c r="D211" s="12">
-        <v>1051</v>
+        <v>929</v>
       </c>
       <c r="E211" s="12">
-        <v>1034</v>
+        <v>929</v>
       </c>
     </row>
     <row r="212" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B212" s="12">
-        <v>7032017</v>
+        <v>16022017</v>
       </c>
       <c r="C212" s="22">
-        <v>0.68310000000000004</v>
+        <v>0.39710000000000001</v>
       </c>
       <c r="D212" s="12">
-        <v>1051</v>
+        <v>1344</v>
       </c>
       <c r="E212" s="12">
-        <v>1034</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="213" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B213" s="12">
-        <v>7032017</v>
+        <v>17022017</v>
       </c>
       <c r="C213" s="22">
-        <v>0.69010000000000005</v>
+        <v>0.42380000000000001</v>
       </c>
       <c r="D213" s="12">
-        <v>1059</v>
+        <v>854</v>
       </c>
       <c r="E213" s="12">
-        <v>1034</v>
+        <v>854</v>
       </c>
     </row>
     <row r="214" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B214" s="12">
-        <v>7032017</v>
+        <v>18022017</v>
       </c>
       <c r="C214" s="22">
-        <v>0.68079999999999996</v>
+        <v>0.53369999999999995</v>
       </c>
       <c r="D214" s="12">
-        <v>1059</v>
+        <v>1706</v>
       </c>
       <c r="E214" s="12">
-        <v>1034</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="215" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B215" s="12">
-        <v>7032017</v>
+        <v>20022017</v>
       </c>
       <c r="C215" s="22">
-        <v>0.67769999999999997</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="D215" s="12">
-        <v>1059</v>
+        <v>1139</v>
       </c>
       <c r="E215" s="12">
-        <v>1034</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="216" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B216" s="12">
         <v>7032017</v>
       </c>
       <c r="C216" s="22">
-        <v>0.67700000000000005</v>
+        <v>0.60119999999999996</v>
       </c>
       <c r="D216" s="12">
-        <v>1104</v>
+        <v>1032</v>
       </c>
       <c r="E216" s="12">
         <v>1034</v>
@@ -21385,101 +21394,101 @@
     </row>
     <row r="217" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B217" s="12">
-        <v>7032017</v>
+        <v>15022017</v>
       </c>
       <c r="C217" s="22">
-        <v>0.67720000000000002</v>
+        <v>0.24390000000000001</v>
       </c>
       <c r="D217" s="12">
-        <v>1104</v>
+        <v>929</v>
       </c>
       <c r="E217" s="12">
-        <v>1034</v>
+        <v>929</v>
       </c>
     </row>
     <row r="218" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B218" s="12">
-        <v>7032017</v>
+        <v>16022017</v>
       </c>
       <c r="C218" s="22">
-        <v>0.67369999999999997</v>
+        <v>0.36930000000000002</v>
       </c>
       <c r="D218" s="12">
-        <v>1104</v>
+        <v>1344</v>
       </c>
       <c r="E218" s="12">
-        <v>1034</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="219" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B219" s="12">
-        <v>7032017</v>
+        <v>17022017</v>
       </c>
       <c r="C219" s="22">
-        <v>0.67700000000000005</v>
+        <v>0.4345</v>
       </c>
       <c r="D219" s="12">
-        <v>1108</v>
+        <v>854</v>
       </c>
       <c r="E219" s="12">
-        <v>1034</v>
+        <v>854</v>
       </c>
     </row>
     <row r="220" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B220" s="12">
-        <v>7032017</v>
+        <v>18022017</v>
       </c>
       <c r="C220" s="22">
-        <v>0.67700000000000005</v>
+        <v>0.4844</v>
       </c>
       <c r="D220" s="12">
-        <v>1108</v>
+        <v>1706</v>
       </c>
       <c r="E220" s="12">
-        <v>1034</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="221" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B221" s="12">
-        <v>7032017</v>
+        <v>20022017</v>
       </c>
       <c r="C221" s="22">
-        <v>0.67979999999999996</v>
+        <v>0.52239999999999998</v>
       </c>
       <c r="D221" s="12">
-        <v>1108</v>
+        <v>1139</v>
       </c>
       <c r="E221" s="12">
-        <v>1034</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="222" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B222" s="12">
         <v>7032017</v>
       </c>
       <c r="C222" s="22">
-        <v>0.59819999999999995</v>
+        <v>0.59870000000000001</v>
       </c>
       <c r="D222" s="12">
-        <v>1112</v>
+        <v>1032</v>
       </c>
       <c r="E222" s="12">
         <v>1034</v>
@@ -21487,103 +21496,107 @@
     </row>
     <row r="223" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="B223" s="12">
-        <v>7032017</v>
+        <v>15022017</v>
       </c>
       <c r="C223" s="22">
-        <v>0.59819999999999995</v>
+        <v>0.24390000000000001</v>
       </c>
       <c r="D223" s="12">
-        <v>1112</v>
+        <v>929</v>
       </c>
       <c r="E223" s="12">
-        <v>1034</v>
+        <v>929</v>
       </c>
     </row>
     <row r="224" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B224" s="12">
-        <v>7032017</v>
+        <v>16022017</v>
       </c>
       <c r="C224" s="22">
-        <v>0.59819999999999995</v>
+        <v>0.36630000000000001</v>
       </c>
       <c r="D224" s="12">
-        <v>1112</v>
+        <v>1344</v>
       </c>
       <c r="E224" s="12">
-        <v>1034</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="225" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B225" s="12">
-        <v>7032017</v>
+        <v>17022017</v>
       </c>
       <c r="C225" s="22">
-        <v>0.73280000000000001</v>
+        <v>0.43990000000000001</v>
       </c>
       <c r="D225" s="12">
-        <v>1115</v>
+        <v>854</v>
       </c>
       <c r="E225" s="12">
-        <v>1034</v>
+        <v>854</v>
       </c>
     </row>
     <row r="226" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B226" s="12">
-        <v>7032017</v>
+        <v>18022017</v>
       </c>
       <c r="C226" s="22">
-        <v>0.73280000000000001</v>
+        <v>0.4844</v>
       </c>
       <c r="D226" s="12">
-        <v>1115</v>
+        <v>1706</v>
       </c>
       <c r="E226" s="12">
-        <v>1034</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="227" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B227" s="12">
-        <v>7032017</v>
+        <v>20022017</v>
       </c>
       <c r="C227" s="22">
-        <v>0.73280000000000001</v>
+        <v>0.52059999999999995</v>
       </c>
       <c r="D227" s="12">
-        <v>1115</v>
+        <v>1139</v>
       </c>
       <c r="E227" s="12">
-        <v>1034</v>
+        <v>1052</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:E227">
+    <sortCondition ref="A3:A227"/>
+    <sortCondition ref="B3:B227"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21777,6 +21790,20 @@
         <v>138</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add export tables and R code for export in thermal hydrolysis
</commit_message>
<xml_diff>
--- a/experiments/thermal hydrolysis/data/BMP2.xlsx
+++ b/experiments/thermal hydrolysis/data/BMP2.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Comp" sheetId="3" r:id="rId3"/>
     <sheet name="ChangeLog" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -291,9 +291,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
@@ -507,6 +504,24 @@
   </si>
   <si>
     <t>Change first B3 to B2 in comp data sheet for 07032017</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>25.02.2019</t>
+  </si>
+  <si>
+    <t>Change cellulose substrates to L (C1, C2, C3 --&gt; L1, L2, L3)</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1038,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,46 +1054,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>86</v>
-      </c>
       <c r="C1" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="L1" s="17" t="s">
-        <v>118</v>
-      </c>
       <c r="M1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1089,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>2</v>
@@ -1101,25 +1116,25 @@
         <v>4</v>
       </c>
       <c r="G2" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N2" s="18" t="s">
         <v>7</v>
@@ -1133,7 +1148,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="16">
         <v>248.94</v>
@@ -1169,7 +1184,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="16">
         <v>257.82</v>
@@ -1205,7 +1220,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="16">
         <v>248.9</v>
@@ -2558,10 +2573,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>53</v>
@@ -2603,10 +2618,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>53</v>
@@ -2648,10 +2663,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>53</v>
@@ -2701,8 +2716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K488"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:I86"/>
+    <sheetView topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E202" sqref="E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,34 +2738,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>59</v>
@@ -2767,7 +2782,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>58</v>
@@ -2776,7 +2791,7 @@
         <v>60</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>61</v>
@@ -5515,7 +5530,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B87" s="12">
         <v>7032017</v>
@@ -5547,7 +5562,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B88" s="12">
         <v>14022017</v>
@@ -5579,7 +5594,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B89" s="12">
         <v>15022017</v>
@@ -5611,7 +5626,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B90" s="12">
         <v>16022017</v>
@@ -5643,7 +5658,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B91" s="12">
         <v>16042017</v>
@@ -5675,7 +5690,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B92" s="12">
         <v>17022017</v>
@@ -5708,7 +5723,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B93" s="12">
         <v>18022017</v>
@@ -5741,7 +5756,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B94" s="12">
         <v>19022017</v>
@@ -5774,7 +5789,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B95" s="12">
         <v>20022017</v>
@@ -5806,7 +5821,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B96" s="12">
         <v>23022017</v>
@@ -7300,7 +7315,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B142" s="12">
         <v>7032017</v>
@@ -7332,7 +7347,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B143" s="12">
         <v>14022017</v>
@@ -7364,7 +7379,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B144" s="12">
         <v>15022017</v>
@@ -7396,7 +7411,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B145" s="12">
         <v>16022017</v>
@@ -7428,7 +7443,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B146" s="12">
         <v>16042017</v>
@@ -7460,7 +7475,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B147" s="12">
         <v>17022017</v>
@@ -7492,7 +7507,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B148" s="12">
         <v>18022017</v>
@@ -7525,7 +7540,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B149" s="12">
         <v>19022017</v>
@@ -7558,7 +7573,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B150" s="12">
         <v>20022017</v>
@@ -7590,7 +7605,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B151" s="12">
         <v>23022017</v>
@@ -9083,7 +9098,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B197" s="12">
         <v>7032017</v>
@@ -9115,7 +9130,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B198" s="12">
         <v>14022017</v>
@@ -9147,7 +9162,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B199" s="12">
         <v>15022017</v>
@@ -9179,7 +9194,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B200" s="12">
         <v>16022017</v>
@@ -9211,7 +9226,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B201" s="12">
         <v>16042017</v>
@@ -9243,7 +9258,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B202" s="12">
         <v>17022017</v>
@@ -9275,7 +9290,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B203" s="12">
         <v>18022017</v>
@@ -9308,7 +9323,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B204" s="12">
         <v>19022017</v>
@@ -9341,7 +9356,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B205" s="12">
         <v>20022017</v>
@@ -9373,7 +9388,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B206" s="12">
         <v>23022017</v>
@@ -17707,8 +17722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E227"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17722,19 +17737,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -17745,10 +17760,10 @@
         <v>56</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>58</v>
@@ -18470,7 +18485,7 @@
     </row>
     <row r="45" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B45" s="12">
         <v>7032017</v>
@@ -18487,7 +18502,7 @@
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B46" s="12">
         <v>15022017</v>
@@ -18504,7 +18519,7 @@
     </row>
     <row r="47" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B47" s="12">
         <v>16022017</v>
@@ -18521,7 +18536,7 @@
     </row>
     <row r="48" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B48" s="12">
         <v>17022017</v>
@@ -18538,7 +18553,7 @@
     </row>
     <row r="49" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B49" s="12">
         <v>18022017</v>
@@ -18555,7 +18570,7 @@
     </row>
     <row r="50" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B50" s="12">
         <v>19022017</v>
@@ -18572,7 +18587,7 @@
     </row>
     <row r="51" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B51" s="12">
         <v>20022017</v>
@@ -18946,7 +18961,7 @@
     </row>
     <row r="73" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B73" s="12">
         <v>7032017</v>
@@ -18963,7 +18978,7 @@
     </row>
     <row r="74" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B74" s="12">
         <v>15022017</v>
@@ -18980,7 +18995,7 @@
     </row>
     <row r="75" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B75" s="12">
         <v>16022017</v>
@@ -18997,7 +19012,7 @@
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B76" s="12">
         <v>17022017</v>
@@ -19014,7 +19029,7 @@
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B77" s="12">
         <v>18022017</v>
@@ -19031,7 +19046,7 @@
     </row>
     <row r="78" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B78" s="12">
         <v>19022017</v>
@@ -19048,7 +19063,7 @@
     </row>
     <row r="79" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B79" s="12">
         <v>20022017</v>
@@ -19422,7 +19437,7 @@
     </row>
     <row r="101" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B101" s="12">
         <v>7032017</v>
@@ -19439,7 +19454,7 @@
     </row>
     <row r="102" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B102" s="12">
         <v>15022017</v>
@@ -19456,7 +19471,7 @@
     </row>
     <row r="103" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B103" s="12">
         <v>16022017</v>
@@ -19473,7 +19488,7 @@
     </row>
     <row r="104" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B104" s="12">
         <v>17022017</v>
@@ -19490,7 +19505,7 @@
     </row>
     <row r="105" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B105" s="12">
         <v>18022017</v>
@@ -19507,7 +19522,7 @@
     </row>
     <row r="106" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B106" s="12">
         <v>19022017</v>
@@ -19524,7 +19539,7 @@
     </row>
     <row r="107" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B107" s="12">
         <v>20022017</v>
@@ -21593,10 +21608,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21611,13 +21626,13 @@
         <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -21625,88 +21640,88 @@
         <v>23092018</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="13"/>
       <c r="D18" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -21717,7 +21732,7 @@
       <c r="B20"/>
       <c r="C20" s="10"/>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -21726,7 +21741,7 @@
     <row r="21" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="13"/>
       <c r="D21" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -21734,74 +21749,88 @@
         <v>30102018</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="15" t="s">
         <v>132</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>137</v>
-      </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
         <v>139</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>141</v>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new descrip column to thermal hydrolysis
</commit_message>
<xml_diff>
--- a/experiments/thermal hydrolysis/data/BMP2.xlsx
+++ b/experiments/thermal hydrolysis/data/BMP2.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -522,6 +522,39 @@
   </si>
   <si>
     <t>Change cellulose substrates to L (C1, C2, C3 --&gt; L1, L2, L3)</t>
+  </si>
+  <si>
+    <t>descrip1</t>
+  </si>
+  <si>
+    <t>Sludge C1</t>
+  </si>
+  <si>
+    <t>Sludge C2</t>
+  </si>
+  <si>
+    <t>Sludge C3</t>
+  </si>
+  <si>
+    <t>Sludge C4</t>
+  </si>
+  <si>
+    <t>Sludge C5</t>
+  </si>
+  <si>
+    <t>Sludge C6</t>
+  </si>
+  <si>
+    <t>Raw sludge</t>
+  </si>
+  <si>
+    <t>Preheated sludge</t>
+  </si>
+  <si>
+    <t>19.03.2019</t>
+  </si>
+  <si>
+    <t>Add new descrip column. Moved old one to descrip1</t>
   </si>
 </sst>
 </file>
@@ -1035,24 +1068,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.85546875" style="16" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.85546875" style="16" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" style="16" customWidth="1"/>
-    <col min="15" max="1023" width="8.5703125" style="16"/>
-    <col min="1024" max="16384" width="9" style="16"/>
+    <col min="4" max="4" width="14.140625" style="16" customWidth="1"/>
+    <col min="5" max="13" width="11.85546875" style="16" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="16" customWidth="1"/>
+    <col min="16" max="1024" width="8.5703125" style="16"/>
+    <col min="1025" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>84</v>
       </c>
@@ -1062,85 +1096,89 @@
       <c r="C1" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>127</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="O2" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
@@ -1150,33 +1188,36 @@
       <c r="C3" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="16">
         <v>248.94</v>
       </c>
-      <c r="G3" s="16">
+      <c r="H3" s="16">
         <v>112.35</v>
-      </c>
-      <c r="H3" s="16">
-        <v>361.3</v>
       </c>
       <c r="I3" s="16">
         <v>361.3</v>
       </c>
-      <c r="J3" s="19">
-        <f t="shared" ref="J3:J38" si="0">AVERAGE(H3:I3)</f>
+      <c r="J3" s="16">
         <v>361.3</v>
       </c>
       <c r="K3" s="19">
-        <f t="shared" ref="K3:K38" si="1">STDEV(H3:I3)</f>
+        <f t="shared" ref="K3:K38" si="0">AVERAGE(I3:J3)</f>
+        <v>361.3</v>
+      </c>
+      <c r="L3" s="19">
+        <f t="shared" ref="L3:L38" si="1">STDEV(I3:J3)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="19">
-        <f t="shared" ref="L3:L38" si="2">321.87-E3-F3-G3+5.534</f>
+      <c r="M3" s="19">
+        <f t="shared" ref="M3:M38" si="2">321.87-F3-G3-H3+5.534</f>
         <v>215.054</v>
       </c>
-      <c r="M3" s="19"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="19"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
@@ -1186,33 +1227,36 @@
       <c r="C4" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="16">
         <v>257.82</v>
       </c>
-      <c r="G4" s="16">
+      <c r="H4" s="16">
         <v>102.26</v>
-      </c>
-      <c r="H4" s="16">
-        <v>360.08</v>
       </c>
       <c r="I4" s="16">
         <v>360.08</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="16">
+        <v>360.08</v>
+      </c>
+      <c r="K4" s="19">
         <f t="shared" si="0"/>
         <v>360.08</v>
       </c>
-      <c r="K4" s="19">
+      <c r="L4" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L4" s="19">
+      <c r="M4" s="19">
         <f t="shared" si="2"/>
         <v>225.14400000000001</v>
       </c>
-      <c r="M4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="19"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -1222,33 +1266,36 @@
       <c r="C5" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="16">
         <v>248.9</v>
       </c>
-      <c r="G5" s="16">
+      <c r="H5" s="16">
         <v>99.58</v>
-      </c>
-      <c r="H5" s="16">
-        <v>348.07</v>
       </c>
       <c r="I5" s="16">
         <v>348.07</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="16">
+        <v>348.07</v>
+      </c>
+      <c r="K5" s="19">
         <f t="shared" si="0"/>
         <v>348.07</v>
       </c>
-      <c r="K5" s="19">
+      <c r="L5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="19">
+      <c r="M5" s="19">
         <f t="shared" si="2"/>
         <v>227.82400000000001</v>
       </c>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="19"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -1258,33 +1305,36 @@
       <c r="C6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="16">
         <v>255.78</v>
       </c>
-      <c r="E6" s="16">
+      <c r="F6" s="16">
         <v>98.96</v>
-      </c>
-      <c r="H6" s="16">
-        <v>354.72</v>
       </c>
       <c r="I6" s="16">
         <v>354.72</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="16">
+        <v>354.72</v>
+      </c>
+      <c r="K6" s="19">
         <f t="shared" si="0"/>
         <v>354.72</v>
       </c>
-      <c r="K6" s="19">
+      <c r="L6" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="19">
+      <c r="M6" s="19">
         <f t="shared" si="2"/>
         <v>228.44400000000002</v>
       </c>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
@@ -1294,33 +1344,36 @@
       <c r="C7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="16">
         <v>257.48</v>
       </c>
-      <c r="E7" s="16">
+      <c r="F7" s="16">
         <v>100.39</v>
-      </c>
-      <c r="H7" s="16">
-        <v>357.83</v>
       </c>
       <c r="I7" s="16">
         <v>357.83</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="16">
+        <v>357.83</v>
+      </c>
+      <c r="K7" s="19">
         <f t="shared" si="0"/>
         <v>357.83</v>
       </c>
-      <c r="K7" s="19">
+      <c r="L7" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="19">
+      <c r="M7" s="19">
         <f t="shared" si="2"/>
         <v>227.01400000000001</v>
       </c>
-      <c r="M7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1330,33 +1383,36 @@
       <c r="C8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="16">
         <v>257.17</v>
       </c>
-      <c r="E8" s="16">
+      <c r="F8" s="16">
         <v>100.48</v>
       </c>
-      <c r="H8" s="16">
+      <c r="I8" s="16">
         <v>357.61</v>
       </c>
-      <c r="I8" s="16">
+      <c r="J8" s="16">
         <v>357.62</v>
       </c>
-      <c r="J8" s="19">
+      <c r="K8" s="19">
         <f t="shared" si="0"/>
         <v>357.61500000000001</v>
       </c>
-      <c r="K8" s="19">
+      <c r="L8" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L8" s="19">
+      <c r="M8" s="19">
         <f t="shared" si="2"/>
         <v>226.92399999999998</v>
       </c>
-      <c r="M8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
@@ -1366,42 +1422,45 @@
       <c r="C9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="16">
         <v>257.39</v>
       </c>
-      <c r="E9" s="16">
+      <c r="F9" s="16">
         <v>101.39</v>
       </c>
-      <c r="F9" s="16">
+      <c r="G9" s="16">
         <v>50.86</v>
-      </c>
-      <c r="H9" s="16">
-        <v>409.53</v>
       </c>
       <c r="I9" s="16">
         <v>409.53</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="16">
+        <v>409.53</v>
+      </c>
+      <c r="K9" s="19">
         <f t="shared" si="0"/>
         <v>409.53</v>
       </c>
-      <c r="K9" s="19">
+      <c r="L9" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="19">
+      <c r="M9" s="19">
         <f t="shared" si="2"/>
         <v>175.154</v>
       </c>
-      <c r="M9" s="20">
+      <c r="N9" s="20">
         <v>64.080399999999997</v>
       </c>
-      <c r="N9" s="21">
-        <f t="shared" ref="N9:N38" si="3">M9/1000*F9</f>
+      <c r="O9" s="21">
+        <f t="shared" ref="O9:O38" si="3">N9/1000*G9</f>
         <v>3.2591291439999996</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
@@ -1411,42 +1470,45 @@
       <c r="C10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="16">
         <v>257.10000000000002</v>
       </c>
-      <c r="E10" s="16">
+      <c r="F10" s="16">
         <v>99.93</v>
       </c>
-      <c r="F10" s="16">
+      <c r="G10" s="16">
         <v>53.6</v>
       </c>
-      <c r="H10" s="16">
+      <c r="I10" s="16">
         <v>410.62</v>
       </c>
-      <c r="I10" s="16">
+      <c r="J10" s="16">
         <v>410.61</v>
       </c>
-      <c r="J10" s="19">
+      <c r="K10" s="19">
         <f t="shared" si="0"/>
         <v>410.61500000000001</v>
       </c>
-      <c r="K10" s="19">
+      <c r="L10" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L10" s="19">
+      <c r="M10" s="19">
         <f t="shared" si="2"/>
         <v>173.874</v>
       </c>
-      <c r="M10" s="20">
+      <c r="N10" s="20">
         <v>64.080399999999997</v>
       </c>
-      <c r="N10" s="21">
+      <c r="O10" s="21">
         <f t="shared" si="3"/>
         <v>3.4347094399999998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>19</v>
       </c>
@@ -1456,42 +1518,45 @@
       <c r="C11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="16">
         <v>234.47</v>
       </c>
-      <c r="E11" s="16">
+      <c r="F11" s="16">
         <v>100.13</v>
       </c>
-      <c r="F11" s="16">
+      <c r="G11" s="16">
         <v>50.13</v>
       </c>
-      <c r="H11" s="16">
+      <c r="I11" s="16">
         <v>384.73</v>
       </c>
-      <c r="I11" s="16">
+      <c r="J11" s="16">
         <v>384.72</v>
       </c>
-      <c r="J11" s="19">
+      <c r="K11" s="19">
         <f t="shared" si="0"/>
         <v>384.72500000000002</v>
       </c>
-      <c r="K11" s="19">
+      <c r="L11" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L11" s="19">
+      <c r="M11" s="19">
         <f t="shared" si="2"/>
         <v>177.14400000000001</v>
       </c>
-      <c r="M11" s="20">
+      <c r="N11" s="20">
         <v>64.080399999999997</v>
       </c>
-      <c r="N11" s="21">
+      <c r="O11" s="21">
         <f t="shared" si="3"/>
         <v>3.2123504519999999</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
@@ -1501,42 +1566,45 @@
       <c r="C12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="16">
         <v>248.38</v>
       </c>
-      <c r="E12" s="16">
+      <c r="F12" s="16">
         <v>101.18</v>
       </c>
-      <c r="F12" s="16">
+      <c r="G12" s="16">
         <v>46.78</v>
       </c>
-      <c r="H12" s="16">
+      <c r="I12" s="16">
         <v>396.28</v>
       </c>
-      <c r="I12" s="16">
+      <c r="J12" s="16">
         <v>396.29</v>
       </c>
-      <c r="J12" s="19">
+      <c r="K12" s="19">
         <f t="shared" si="0"/>
         <v>396.28499999999997</v>
       </c>
-      <c r="K12" s="19">
+      <c r="L12" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118992383E-3</v>
       </c>
-      <c r="L12" s="19">
+      <c r="M12" s="19">
         <f t="shared" si="2"/>
         <v>179.44399999999999</v>
       </c>
-      <c r="M12" s="20">
+      <c r="N12" s="20">
         <v>69.671499999999995</v>
       </c>
-      <c r="N12" s="21">
+      <c r="O12" s="21">
         <f t="shared" si="3"/>
         <v>3.2592327700000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>22</v>
       </c>
@@ -1546,42 +1614,45 @@
       <c r="C13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="16">
         <v>257.06</v>
       </c>
-      <c r="E13" s="16">
+      <c r="F13" s="16">
         <v>100.61</v>
       </c>
-      <c r="F13" s="16">
+      <c r="G13" s="16">
         <v>49.95</v>
-      </c>
-      <c r="H13" s="16">
-        <v>407.58</v>
       </c>
       <c r="I13" s="16">
         <v>407.58</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="16">
+        <v>407.58</v>
+      </c>
+      <c r="K13" s="19">
         <f t="shared" si="0"/>
         <v>407.58</v>
       </c>
-      <c r="K13" s="19">
+      <c r="L13" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L13" s="19">
+      <c r="M13" s="19">
         <f t="shared" si="2"/>
         <v>176.84399999999999</v>
       </c>
-      <c r="M13" s="20">
+      <c r="N13" s="20">
         <v>69.671499999999995</v>
       </c>
-      <c r="N13" s="21">
+      <c r="O13" s="21">
         <f t="shared" si="3"/>
         <v>3.4800914249999999</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>23</v>
       </c>
@@ -1591,42 +1662,45 @@
       <c r="C14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="16">
         <v>255.5</v>
       </c>
-      <c r="E14" s="16">
+      <c r="F14" s="16">
         <v>102.71</v>
       </c>
-      <c r="F14" s="16">
+      <c r="G14" s="16">
         <v>46.8</v>
       </c>
-      <c r="H14" s="16">
+      <c r="I14" s="16">
         <v>404.93</v>
       </c>
-      <c r="I14" s="16">
+      <c r="J14" s="16">
         <v>404.94</v>
       </c>
-      <c r="J14" s="19">
+      <c r="K14" s="19">
         <f t="shared" si="0"/>
         <v>404.935</v>
       </c>
-      <c r="K14" s="19">
+      <c r="L14" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L14" s="19">
+      <c r="M14" s="19">
         <f t="shared" si="2"/>
         <v>177.89400000000001</v>
       </c>
-      <c r="M14" s="20">
+      <c r="N14" s="20">
         <v>69.671499999999995</v>
       </c>
-      <c r="N14" s="21">
+      <c r="O14" s="21">
         <f t="shared" si="3"/>
         <v>3.2606261999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>24</v>
       </c>
@@ -1636,42 +1710,45 @@
       <c r="C15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="16">
         <v>256.51</v>
       </c>
-      <c r="E15" s="16">
+      <c r="F15" s="16">
         <v>101.69</v>
       </c>
-      <c r="F15" s="16">
+      <c r="G15" s="16">
         <v>44.15</v>
       </c>
-      <c r="H15" s="16">
+      <c r="I15" s="16">
         <v>402.31</v>
       </c>
-      <c r="I15" s="16">
+      <c r="J15" s="16">
         <v>402.32</v>
       </c>
-      <c r="J15" s="19">
+      <c r="K15" s="19">
         <f t="shared" si="0"/>
         <v>402.315</v>
       </c>
-      <c r="K15" s="19">
+      <c r="L15" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L15" s="19">
+      <c r="M15" s="19">
         <f t="shared" si="2"/>
         <v>181.56399999999999</v>
       </c>
-      <c r="M15" s="20">
+      <c r="N15" s="20">
         <v>75.610699999999994</v>
       </c>
-      <c r="N15" s="21">
+      <c r="O15" s="21">
         <f t="shared" si="3"/>
         <v>3.3382124049999993</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
@@ -1681,42 +1758,45 @@
       <c r="C16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="16">
         <v>257.49</v>
       </c>
-      <c r="E16" s="16">
+      <c r="F16" s="16">
         <v>102.82</v>
       </c>
-      <c r="F16" s="16">
+      <c r="G16" s="16">
         <v>43.84</v>
       </c>
-      <c r="H16" s="16">
+      <c r="I16" s="16">
         <v>404.12</v>
       </c>
-      <c r="I16" s="16">
+      <c r="J16" s="16">
         <v>404.11</v>
       </c>
-      <c r="J16" s="19">
+      <c r="K16" s="19">
         <f t="shared" si="0"/>
         <v>404.11500000000001</v>
       </c>
-      <c r="K16" s="19">
+      <c r="L16" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L16" s="19">
+      <c r="M16" s="19">
         <f t="shared" si="2"/>
         <v>180.744</v>
       </c>
-      <c r="M16" s="20">
+      <c r="N16" s="20">
         <v>75.610699999999994</v>
       </c>
-      <c r="N16" s="21">
+      <c r="O16" s="21">
         <f t="shared" si="3"/>
         <v>3.3147730879999999</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -1726,42 +1806,45 @@
       <c r="C17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="16">
         <v>257.8</v>
       </c>
-      <c r="E17" s="16">
+      <c r="F17" s="16">
         <v>101.3</v>
       </c>
-      <c r="F17" s="16">
+      <c r="G17" s="16">
         <v>42.81</v>
       </c>
-      <c r="H17" s="16">
+      <c r="I17" s="16">
         <v>401.85</v>
       </c>
-      <c r="I17" s="16">
+      <c r="J17" s="16">
         <v>401.86</v>
       </c>
-      <c r="J17" s="19">
+      <c r="K17" s="19">
         <f t="shared" si="0"/>
         <v>401.85500000000002</v>
       </c>
-      <c r="K17" s="19">
+      <c r="L17" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L17" s="19">
+      <c r="M17" s="19">
         <f t="shared" si="2"/>
         <v>183.29399999999998</v>
       </c>
-      <c r="M17" s="20">
+      <c r="N17" s="20">
         <v>75.610699999999994</v>
       </c>
-      <c r="N17" s="21">
+      <c r="O17" s="21">
         <f t="shared" si="3"/>
         <v>3.2368940669999997</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
@@ -1771,42 +1854,45 @@
       <c r="C18" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="16">
         <v>248.33</v>
       </c>
-      <c r="E18" s="16">
+      <c r="F18" s="16">
         <v>99.89</v>
       </c>
-      <c r="F18" s="16">
+      <c r="G18" s="16">
         <v>43.48</v>
-      </c>
-      <c r="H18" s="16">
-        <v>391.69</v>
       </c>
       <c r="I18" s="16">
         <v>391.69</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="16">
+        <v>391.69</v>
+      </c>
+      <c r="K18" s="19">
         <f t="shared" si="0"/>
         <v>391.69</v>
       </c>
-      <c r="K18" s="19">
+      <c r="L18" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L18" s="19">
+      <c r="M18" s="19">
         <f t="shared" si="2"/>
         <v>184.03400000000002</v>
       </c>
-      <c r="M18" s="20">
+      <c r="N18" s="20">
         <v>77.304699999999997</v>
       </c>
-      <c r="N18" s="21">
+      <c r="O18" s="21">
         <f t="shared" si="3"/>
         <v>3.3612083559999992</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>30</v>
       </c>
@@ -1816,42 +1902,45 @@
       <c r="C19" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="16">
         <v>234.42</v>
       </c>
-      <c r="E19" s="16">
+      <c r="F19" s="16">
         <v>100.53</v>
       </c>
-      <c r="F19" s="16">
+      <c r="G19" s="16">
         <v>42.62</v>
-      </c>
-      <c r="H19" s="16">
-        <v>377.52</v>
       </c>
       <c r="I19" s="16">
         <v>377.52</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="16">
+        <v>377.52</v>
+      </c>
+      <c r="K19" s="19">
         <f t="shared" si="0"/>
         <v>377.52</v>
       </c>
-      <c r="K19" s="19">
+      <c r="L19" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L19" s="19">
+      <c r="M19" s="19">
         <f t="shared" si="2"/>
         <v>184.25399999999999</v>
       </c>
-      <c r="M19" s="20">
+      <c r="N19" s="20">
         <v>77.304699999999997</v>
       </c>
-      <c r="N19" s="21">
+      <c r="O19" s="21">
         <f t="shared" si="3"/>
         <v>3.2947263139999996</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>31</v>
       </c>
@@ -1861,42 +1950,45 @@
       <c r="C20" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="16">
         <v>257.01</v>
       </c>
-      <c r="E20" s="16">
+      <c r="F20" s="16">
         <v>100.29</v>
       </c>
-      <c r="F20" s="16">
+      <c r="G20" s="16">
         <v>42.92</v>
       </c>
-      <c r="H20" s="16">
+      <c r="I20" s="16">
         <v>400.18</v>
       </c>
-      <c r="I20" s="16">
+      <c r="J20" s="16">
         <v>400.19</v>
       </c>
-      <c r="J20" s="19">
+      <c r="K20" s="19">
         <f t="shared" si="0"/>
         <v>400.185</v>
       </c>
-      <c r="K20" s="19">
+      <c r="L20" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L20" s="19">
+      <c r="M20" s="19">
         <f t="shared" si="2"/>
         <v>184.19399999999996</v>
       </c>
-      <c r="M20" s="20">
+      <c r="N20" s="20">
         <v>77.304699999999997</v>
       </c>
-      <c r="N20" s="21">
+      <c r="O20" s="21">
         <f t="shared" si="3"/>
         <v>3.3179177239999995</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>32</v>
       </c>
@@ -1906,42 +1998,45 @@
       <c r="C21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="16">
         <v>257.51</v>
       </c>
-      <c r="E21" s="16">
+      <c r="F21" s="16">
         <v>101.72</v>
       </c>
-      <c r="F21" s="16">
+      <c r="G21" s="16">
         <v>39.79</v>
       </c>
-      <c r="H21" s="16">
+      <c r="I21" s="16">
         <v>398.95</v>
       </c>
-      <c r="I21" s="16">
+      <c r="J21" s="16">
         <v>398.94</v>
       </c>
-      <c r="J21" s="19">
+      <c r="K21" s="19">
         <f t="shared" si="0"/>
         <v>398.94499999999999</v>
       </c>
-      <c r="K21" s="19">
+      <c r="L21" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L21" s="19">
+      <c r="M21" s="19">
         <f t="shared" si="2"/>
         <v>185.89400000000001</v>
       </c>
-      <c r="M21" s="20">
+      <c r="N21" s="20">
         <v>81.534199999999998</v>
       </c>
-      <c r="N21" s="21">
+      <c r="O21" s="21">
         <f t="shared" si="3"/>
         <v>3.244245818</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>34</v>
       </c>
@@ -1951,42 +2046,45 @@
       <c r="C22" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="16">
         <v>258.04000000000002</v>
       </c>
-      <c r="E22" s="16">
+      <c r="F22" s="16">
         <v>107.63</v>
       </c>
-      <c r="F22" s="16">
+      <c r="G22" s="16">
         <v>41.63</v>
       </c>
-      <c r="H22" s="16">
+      <c r="I22" s="16">
         <v>407.23</v>
       </c>
-      <c r="I22" s="16">
+      <c r="J22" s="16">
         <v>407.24</v>
       </c>
-      <c r="J22" s="19">
+      <c r="K22" s="19">
         <f t="shared" si="0"/>
         <v>407.23500000000001</v>
       </c>
-      <c r="K22" s="19">
+      <c r="L22" s="19">
         <f t="shared" si="1"/>
         <v>7.0710678118590439E-3</v>
       </c>
-      <c r="L22" s="19">
+      <c r="M22" s="19">
         <f t="shared" si="2"/>
         <v>178.14400000000001</v>
       </c>
-      <c r="M22" s="20">
+      <c r="N22" s="20">
         <v>81.534199999999998</v>
       </c>
-      <c r="N22" s="21">
+      <c r="O22" s="21">
         <f t="shared" si="3"/>
         <v>3.3942687460000003</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>35</v>
       </c>
@@ -1996,42 +2094,45 @@
       <c r="C23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="16">
         <v>257.5</v>
       </c>
-      <c r="E23" s="16">
+      <c r="F23" s="16">
         <v>102.14</v>
       </c>
-      <c r="F23" s="16">
+      <c r="G23" s="16">
         <v>39.799999999999997</v>
-      </c>
-      <c r="H23" s="16">
-        <v>399.38</v>
       </c>
       <c r="I23" s="16">
         <v>399.38</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="16">
+        <v>399.38</v>
+      </c>
+      <c r="K23" s="19">
         <f t="shared" si="0"/>
         <v>399.38</v>
       </c>
-      <c r="K23" s="19">
+      <c r="L23" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L23" s="19">
+      <c r="M23" s="19">
         <f t="shared" si="2"/>
         <v>185.464</v>
       </c>
-      <c r="M23" s="20">
+      <c r="N23" s="20">
         <v>81.534199999999998</v>
       </c>
-      <c r="N23" s="21">
+      <c r="O23" s="21">
         <f t="shared" si="3"/>
         <v>3.2450611599999997</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
@@ -2041,42 +2142,45 @@
       <c r="C24" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="16">
         <v>248.49</v>
       </c>
-      <c r="E24" s="16">
+      <c r="F24" s="16">
         <v>103.03</v>
       </c>
-      <c r="F24" s="16">
+      <c r="G24" s="16">
         <v>39.46</v>
-      </c>
-      <c r="H24" s="16">
-        <v>390.92</v>
       </c>
       <c r="I24" s="16">
         <v>390.92</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="16">
+        <v>390.92</v>
+      </c>
+      <c r="K24" s="19">
         <f t="shared" si="0"/>
         <v>390.92</v>
       </c>
-      <c r="K24" s="19">
+      <c r="L24" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L24" s="19">
+      <c r="M24" s="19">
         <f t="shared" si="2"/>
         <v>184.91399999999999</v>
       </c>
-      <c r="M24" s="20">
+      <c r="N24" s="20">
         <v>82.914000000000001</v>
       </c>
-      <c r="N24" s="21">
+      <c r="O24" s="21">
         <f t="shared" si="3"/>
         <v>3.2717864400000001</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>38</v>
       </c>
@@ -2086,42 +2190,45 @@
       <c r="C25" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="16">
         <v>255.87</v>
       </c>
-      <c r="E25" s="16">
+      <c r="F25" s="16">
         <v>99.26</v>
       </c>
-      <c r="F25" s="16">
+      <c r="G25" s="16">
         <v>38.630000000000003</v>
-      </c>
-      <c r="H25" s="16">
-        <v>393.73</v>
       </c>
       <c r="I25" s="16">
         <v>393.73</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="16">
+        <v>393.73</v>
+      </c>
+      <c r="K25" s="19">
         <f t="shared" si="0"/>
         <v>393.73</v>
       </c>
-      <c r="K25" s="19">
+      <c r="L25" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L25" s="19">
+      <c r="M25" s="19">
         <f t="shared" si="2"/>
         <v>189.51400000000001</v>
       </c>
-      <c r="M25" s="20">
+      <c r="N25" s="20">
         <v>82.914000000000001</v>
       </c>
-      <c r="N25" s="21">
+      <c r="O25" s="21">
         <f t="shared" si="3"/>
         <v>3.2029678200000005</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
@@ -2131,42 +2238,45 @@
       <c r="C26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="16">
         <v>257.27999999999997</v>
       </c>
-      <c r="E26" s="16">
+      <c r="F26" s="16">
         <v>100.51</v>
       </c>
-      <c r="F26" s="16">
+      <c r="G26" s="16">
         <v>39.01</v>
-      </c>
-      <c r="H26" s="16">
-        <v>396.75</v>
       </c>
       <c r="I26" s="16">
         <v>396.75</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="16">
+        <v>396.75</v>
+      </c>
+      <c r="K26" s="19">
         <f t="shared" si="0"/>
         <v>396.75</v>
       </c>
-      <c r="K26" s="19">
+      <c r="L26" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L26" s="19">
+      <c r="M26" s="19">
         <f t="shared" si="2"/>
         <v>187.88400000000001</v>
       </c>
-      <c r="M26" s="20">
+      <c r="N26" s="20">
         <v>82.914000000000001</v>
       </c>
-      <c r="N26" s="21">
+      <c r="O26" s="21">
         <f t="shared" si="3"/>
         <v>3.2344751399999998</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>40</v>
       </c>
@@ -2176,42 +2286,45 @@
       <c r="C27" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="16">
         <v>248.44</v>
       </c>
-      <c r="E27" s="16">
+      <c r="F27" s="16">
         <v>101.36</v>
       </c>
-      <c r="F27" s="16">
+      <c r="G27" s="16">
         <v>35.5</v>
-      </c>
-      <c r="H27" s="16">
-        <v>385.27</v>
       </c>
       <c r="I27" s="16">
         <v>385.27</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="16">
+        <v>385.27</v>
+      </c>
+      <c r="K27" s="19">
         <f t="shared" si="0"/>
         <v>385.27</v>
       </c>
-      <c r="K27" s="19">
+      <c r="L27" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L27" s="19">
+      <c r="M27" s="19">
         <f t="shared" si="2"/>
         <v>190.54399999999998</v>
       </c>
-      <c r="M27" s="20">
+      <c r="N27" s="20">
         <v>93.764399999999995</v>
       </c>
-      <c r="N27" s="21">
+      <c r="O27" s="21">
         <f t="shared" si="3"/>
         <v>3.3286362</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>42</v>
       </c>
@@ -2221,42 +2334,45 @@
       <c r="C28" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="16">
         <v>257.13</v>
       </c>
-      <c r="E28" s="16">
+      <c r="F28" s="16">
         <v>100.34</v>
       </c>
-      <c r="F28" s="16">
+      <c r="G28" s="16">
         <v>33.69</v>
-      </c>
-      <c r="H28" s="16">
-        <v>391.09</v>
       </c>
       <c r="I28" s="16">
         <v>391.09</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="16">
+        <v>391.09</v>
+      </c>
+      <c r="K28" s="19">
         <f t="shared" si="0"/>
         <v>391.09</v>
       </c>
-      <c r="K28" s="19">
+      <c r="L28" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L28" s="19">
+      <c r="M28" s="19">
         <f t="shared" si="2"/>
         <v>193.374</v>
       </c>
-      <c r="M28" s="20">
+      <c r="N28" s="20">
         <v>93.764399999999995</v>
       </c>
-      <c r="N28" s="21">
+      <c r="O28" s="21">
         <f t="shared" si="3"/>
         <v>3.1589226359999998</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>43</v>
       </c>
@@ -2266,42 +2382,45 @@
       <c r="C29" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="16">
         <v>254.13</v>
       </c>
-      <c r="E29" s="16">
+      <c r="F29" s="16">
         <v>103.49</v>
       </c>
-      <c r="F29" s="16">
+      <c r="G29" s="16">
         <v>33.6</v>
-      </c>
-      <c r="H29" s="16">
-        <v>391.14</v>
       </c>
       <c r="I29" s="16">
         <v>391.14</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="16">
+        <v>391.14</v>
+      </c>
+      <c r="K29" s="19">
         <f t="shared" si="0"/>
         <v>391.14</v>
       </c>
-      <c r="K29" s="19">
+      <c r="L29" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L29" s="19">
+      <c r="M29" s="19">
         <f t="shared" si="2"/>
         <v>190.31399999999999</v>
       </c>
-      <c r="M29" s="20">
+      <c r="N29" s="20">
         <v>93.764399999999995</v>
       </c>
-      <c r="N29" s="21">
+      <c r="O29" s="21">
         <f t="shared" si="3"/>
         <v>3.1504838400000001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>44</v>
       </c>
@@ -2311,42 +2430,45 @@
       <c r="C30" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="16">
         <v>257.37</v>
       </c>
-      <c r="E30" s="16">
+      <c r="F30" s="16">
         <v>101.41</v>
       </c>
-      <c r="F30" s="16">
+      <c r="G30" s="16">
         <v>29.82</v>
-      </c>
-      <c r="H30" s="16">
-        <v>388.55</v>
       </c>
       <c r="I30" s="16">
         <v>388.55</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="16">
+        <v>388.55</v>
+      </c>
+      <c r="K30" s="19">
         <f t="shared" si="0"/>
         <v>388.55</v>
       </c>
-      <c r="K30" s="19">
+      <c r="L30" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L30" s="19">
+      <c r="M30" s="19">
         <f t="shared" si="2"/>
         <v>196.17400000000001</v>
       </c>
-      <c r="M30" s="20">
+      <c r="N30" s="20">
         <v>107.4922</v>
       </c>
-      <c r="N30" s="21">
+      <c r="O30" s="21">
         <f t="shared" si="3"/>
         <v>3.2054174039999999</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>46</v>
       </c>
@@ -2356,42 +2478,45 @@
       <c r="C31" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="16">
         <v>255.12</v>
       </c>
-      <c r="E31" s="16">
+      <c r="F31" s="16">
         <v>102.59</v>
       </c>
-      <c r="F31" s="16">
+      <c r="G31" s="16">
         <v>29.76</v>
-      </c>
-      <c r="H31" s="16">
-        <v>387.4</v>
       </c>
       <c r="I31" s="16">
         <v>387.4</v>
       </c>
-      <c r="J31" s="19">
+      <c r="J31" s="16">
+        <v>387.4</v>
+      </c>
+      <c r="K31" s="19">
         <f t="shared" si="0"/>
         <v>387.4</v>
       </c>
-      <c r="K31" s="19">
+      <c r="L31" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L31" s="19">
+      <c r="M31" s="19">
         <f t="shared" si="2"/>
         <v>195.054</v>
       </c>
-      <c r="M31" s="20">
+      <c r="N31" s="20">
         <v>107.4922</v>
       </c>
-      <c r="N31" s="21">
+      <c r="O31" s="21">
         <f t="shared" si="3"/>
         <v>3.1989678719999999</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>47</v>
       </c>
@@ -2401,42 +2526,45 @@
       <c r="C32" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="16">
         <v>255.9</v>
       </c>
-      <c r="E32" s="16">
+      <c r="F32" s="16">
         <v>100.25</v>
       </c>
-      <c r="F32" s="16">
+      <c r="G32" s="16">
         <v>29.36</v>
-      </c>
-      <c r="H32" s="16">
-        <v>385.45</v>
       </c>
       <c r="I32" s="16">
         <v>385.45</v>
       </c>
-      <c r="J32" s="19">
+      <c r="J32" s="16">
+        <v>385.45</v>
+      </c>
+      <c r="K32" s="19">
         <f t="shared" si="0"/>
         <v>385.45</v>
       </c>
-      <c r="K32" s="19">
+      <c r="L32" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L32" s="19">
+      <c r="M32" s="19">
         <f t="shared" si="2"/>
         <v>197.79399999999998</v>
       </c>
-      <c r="M32" s="20">
+      <c r="N32" s="20">
         <v>107.4922</v>
       </c>
-      <c r="N32" s="21">
+      <c r="O32" s="21">
         <f t="shared" si="3"/>
         <v>3.1559709919999999</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>48</v>
       </c>
@@ -2446,42 +2574,45 @@
       <c r="C33" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="16">
         <v>255.81</v>
       </c>
-      <c r="E33" s="16">
+      <c r="F33" s="16">
         <v>100.67</v>
       </c>
-      <c r="F33" s="16">
+      <c r="G33" s="16">
         <v>0.61</v>
-      </c>
-      <c r="H33" s="16">
-        <v>357.05</v>
       </c>
       <c r="I33" s="16">
         <v>357.05</v>
       </c>
-      <c r="J33" s="19">
+      <c r="J33" s="16">
+        <v>357.05</v>
+      </c>
+      <c r="K33" s="19">
         <f t="shared" si="0"/>
         <v>357.05</v>
       </c>
-      <c r="K33" s="19">
+      <c r="L33" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L33" s="19">
+      <c r="M33" s="19">
         <f t="shared" si="2"/>
         <v>226.12399999999997</v>
       </c>
-      <c r="M33" s="20">
+      <c r="N33" s="20">
         <v>1000</v>
       </c>
-      <c r="N33" s="21">
+      <c r="O33" s="21">
         <f t="shared" si="3"/>
         <v>0.61</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>50</v>
       </c>
@@ -2491,42 +2622,45 @@
       <c r="C34" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="16">
         <v>248.2</v>
       </c>
-      <c r="E34" s="16">
+      <c r="F34" s="16">
         <v>100.36</v>
       </c>
-      <c r="F34" s="16">
+      <c r="G34" s="16">
         <v>0.61</v>
-      </c>
-      <c r="H34" s="16">
-        <v>349.14</v>
       </c>
       <c r="I34" s="16">
         <v>349.14</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="16">
+        <v>349.14</v>
+      </c>
+      <c r="K34" s="19">
         <f t="shared" si="0"/>
         <v>349.14</v>
       </c>
-      <c r="K34" s="19">
+      <c r="L34" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L34" s="19">
+      <c r="M34" s="19">
         <f t="shared" si="2"/>
         <v>226.43399999999997</v>
       </c>
-      <c r="M34" s="20">
+      <c r="N34" s="20">
         <v>1000</v>
       </c>
-      <c r="N34" s="21">
+      <c r="O34" s="21">
         <f t="shared" si="3"/>
         <v>0.61</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>51</v>
       </c>
@@ -2536,42 +2670,45 @@
       <c r="C35" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="16">
         <v>256.31</v>
       </c>
-      <c r="E35" s="16">
+      <c r="F35" s="16">
         <v>102.54</v>
       </c>
-      <c r="F35" s="16">
+      <c r="G35" s="16">
         <v>0.61</v>
-      </c>
-      <c r="H35" s="16">
-        <v>359.42</v>
       </c>
       <c r="I35" s="16">
         <v>359.42</v>
       </c>
-      <c r="J35" s="19">
+      <c r="J35" s="16">
+        <v>359.42</v>
+      </c>
+      <c r="K35" s="19">
         <f t="shared" si="0"/>
         <v>359.42</v>
       </c>
-      <c r="K35" s="19">
+      <c r="L35" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L35" s="19">
+      <c r="M35" s="19">
         <f t="shared" si="2"/>
         <v>224.25399999999996</v>
       </c>
-      <c r="M35" s="20">
+      <c r="N35" s="20">
         <v>1000</v>
       </c>
-      <c r="N35" s="21">
+      <c r="O35" s="21">
         <f t="shared" si="3"/>
         <v>0.61</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>142</v>
       </c>
@@ -2581,42 +2718,45 @@
       <c r="C36" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="16">
         <v>255.78</v>
       </c>
-      <c r="E36" s="16">
+      <c r="F36" s="16">
         <v>101.53</v>
       </c>
-      <c r="F36" s="16">
+      <c r="G36" s="16">
         <v>1</v>
-      </c>
-      <c r="H36" s="16">
-        <v>358.26</v>
       </c>
       <c r="I36" s="16">
         <v>358.26</v>
       </c>
-      <c r="J36" s="19">
+      <c r="J36" s="16">
+        <v>358.26</v>
+      </c>
+      <c r="K36" s="19">
         <f t="shared" si="0"/>
         <v>358.26</v>
       </c>
-      <c r="K36" s="19">
+      <c r="L36" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L36" s="19">
+      <c r="M36" s="19">
         <f t="shared" si="2"/>
         <v>224.874</v>
       </c>
-      <c r="M36" s="20">
+      <c r="N36" s="20">
         <v>952</v>
       </c>
-      <c r="N36" s="21">
+      <c r="O36" s="21">
         <f t="shared" si="3"/>
         <v>0.95199999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>143</v>
       </c>
@@ -2626,42 +2766,45 @@
       <c r="C37" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="16">
         <v>257.58999999999997</v>
       </c>
-      <c r="E37" s="16">
+      <c r="F37" s="16">
         <v>101.68</v>
       </c>
-      <c r="F37" s="16">
+      <c r="G37" s="16">
         <v>0.98</v>
-      </c>
-      <c r="H37" s="16">
-        <v>360.2</v>
       </c>
       <c r="I37" s="16">
         <v>360.2</v>
       </c>
-      <c r="J37" s="19">
+      <c r="J37" s="16">
+        <v>360.2</v>
+      </c>
+      <c r="K37" s="19">
         <f t="shared" si="0"/>
         <v>360.2</v>
       </c>
-      <c r="K37" s="19">
+      <c r="L37" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L37" s="19">
+      <c r="M37" s="19">
         <f t="shared" si="2"/>
         <v>224.744</v>
       </c>
-      <c r="M37" s="20">
+      <c r="N37" s="20">
         <v>952</v>
       </c>
-      <c r="N37" s="21">
+      <c r="O37" s="21">
         <f t="shared" si="3"/>
         <v>0.9329599999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>144</v>
       </c>
@@ -2671,37 +2814,40 @@
       <c r="C38" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="16">
         <v>257.69</v>
       </c>
-      <c r="E38" s="16">
+      <c r="F38" s="16">
         <v>102.85</v>
       </c>
-      <c r="F38" s="16">
+      <c r="G38" s="16">
         <v>1.03</v>
-      </c>
-      <c r="H38" s="16">
-        <v>361.51</v>
       </c>
       <c r="I38" s="16">
         <v>361.51</v>
       </c>
-      <c r="J38" s="19">
+      <c r="J38" s="16">
+        <v>361.51</v>
+      </c>
+      <c r="K38" s="19">
         <f t="shared" si="0"/>
         <v>361.51</v>
       </c>
-      <c r="K38" s="19">
+      <c r="L38" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L38" s="19">
+      <c r="M38" s="19">
         <f t="shared" si="2"/>
         <v>223.524</v>
       </c>
-      <c r="M38" s="20">
+      <c r="N38" s="20">
         <v>952</v>
       </c>
-      <c r="N38" s="21">
+      <c r="O38" s="21">
         <f t="shared" si="3"/>
         <v>0.98055999999999999</v>
       </c>
@@ -21608,10 +21754,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21833,6 +21979,20 @@
         <v>146</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change y-axis label on UQ2 xCH4 plot. Work on plots for outline in thermal hydrolysis
</commit_message>
<xml_diff>
--- a/experiments/thermal hydrolysis/data/BMP2.xlsx
+++ b/experiments/thermal hydrolysis/data/BMP2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -1070,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,7 @@
         <v>129</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="E3" s="16">
         <v>248.94</v>
@@ -1228,7 +1228,7 @@
         <v>129</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="E4" s="16">
         <v>257.82</v>
@@ -1267,7 +1267,7 @@
         <v>129</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="E5" s="16">
         <v>248.9</v>
@@ -1306,7 +1306,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E6" s="16">
         <v>255.78</v>
@@ -1345,7 +1345,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E7" s="16">
         <v>257.48</v>
@@ -1384,7 +1384,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E8" s="16">
         <v>257.17</v>
@@ -21756,7 +21756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add round function to supplementary tables for TH
</commit_message>
<xml_diff>
--- a/experiments/thermal hydrolysis/data/BMP2.xlsx
+++ b/experiments/thermal hydrolysis/data/BMP2.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="164">
   <si>
     <t>id</t>
   </si>
@@ -555,6 +555,24 @@
   </si>
   <si>
     <t>Add new descrip column. Moved old one to descrip1</t>
+  </si>
+  <si>
+    <t>Inoculum VS (g)</t>
+  </si>
+  <si>
+    <t>m.inoc.vs</t>
+  </si>
+  <si>
+    <t>conc.inoc.vs</t>
+  </si>
+  <si>
+    <t>Inoculum VS conc (g/kg)</t>
+  </si>
+  <si>
+    <t>02.04.2019</t>
+  </si>
+  <si>
+    <t>Add inoc VS conc and m.inoc.vs column to setup data from Palle Olsens thesis p. 113</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1104,7 @@
     <col min="1025" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>84</v>
       </c>
@@ -1130,8 +1148,14 @@
       <c r="O1" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1177,8 +1201,14 @@
       <c r="O2" s="18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
@@ -1217,7 +1247,7 @@
       </c>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1286,7 @@
       </c>
       <c r="N4" s="19"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -1295,7 +1325,7 @@
       </c>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -1332,9 +1362,17 @@
         <f t="shared" si="2"/>
         <v>228.44400000000002</v>
       </c>
-      <c r="N6" s="19"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="20"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q6" s="16">
+        <f>P6*F6/1000</f>
+        <v>3.2159723920000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
@@ -1371,9 +1409,17 @@
         <f t="shared" si="2"/>
         <v>227.01400000000001</v>
       </c>
-      <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q7" s="16">
+        <f t="shared" ref="Q7:Q38" si="3">P7*F7/1000</f>
+        <v>3.2624441030000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1410,9 +1456,17 @@
         <f t="shared" si="2"/>
         <v>226.92399999999998</v>
       </c>
-      <c r="N8" s="19"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q8" s="16">
+        <f t="shared" si="3"/>
+        <v>3.2653688960000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
@@ -1456,11 +1510,18 @@
         <v>64.080399999999997</v>
       </c>
       <c r="O9" s="21">
-        <f t="shared" ref="O9:O38" si="3">N9/1000*G9</f>
+        <f>N9/1000*G9</f>
         <v>3.2591291439999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q9" s="16">
+        <f t="shared" si="3"/>
+        <v>3.2949418029999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
@@ -1504,11 +1565,18 @@
         <v>64.080399999999997</v>
       </c>
       <c r="O10" s="21">
+        <f t="shared" ref="O9:O38" si="4">N10/1000*G10</f>
+        <v>3.4347094399999998</v>
+      </c>
+      <c r="P10" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q10" s="16">
         <f t="shared" si="3"/>
-        <v>3.4347094399999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2474951610000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>19</v>
       </c>
@@ -1552,11 +1620,18 @@
         <v>64.080399999999997</v>
       </c>
       <c r="O11" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2123504519999999</v>
+      </c>
+      <c r="P11" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q11" s="16">
         <f t="shared" si="3"/>
-        <v>3.2123504519999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2539947009999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
@@ -1600,11 +1675,18 @@
         <v>69.671499999999995</v>
       </c>
       <c r="O12" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2592327700000001</v>
+      </c>
+      <c r="P12" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q12" s="16">
         <f t="shared" si="3"/>
-        <v>3.2592327700000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2881172860000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>22</v>
       </c>
@@ -1648,11 +1730,18 @@
         <v>69.671499999999995</v>
       </c>
       <c r="O13" s="21">
+        <f t="shared" si="4"/>
+        <v>3.4800914249999999</v>
+      </c>
+      <c r="P13" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q13" s="16">
         <f t="shared" si="3"/>
-        <v>3.4800914249999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2695935970000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>23</v>
       </c>
@@ -1696,11 +1785,18 @@
         <v>69.671499999999995</v>
       </c>
       <c r="O14" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2606261999999995</v>
+      </c>
+      <c r="P14" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q14" s="16">
         <f t="shared" si="3"/>
-        <v>3.2606261999999995</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.337838767</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>24</v>
       </c>
@@ -1744,11 +1840,18 @@
         <v>75.610699999999994</v>
       </c>
       <c r="O15" s="21">
+        <f t="shared" si="4"/>
+        <v>3.3382124049999993</v>
+      </c>
+      <c r="P15" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q15" s="16">
         <f t="shared" si="3"/>
-        <v>3.3382124049999993</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3046911130000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
@@ -1792,11 +1895,18 @@
         <v>75.610699999999994</v>
       </c>
       <c r="O16" s="21">
+        <f t="shared" si="4"/>
+        <v>3.3147730879999999</v>
+      </c>
+      <c r="P16" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q16" s="16">
         <f t="shared" si="3"/>
-        <v>3.3147730879999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3414135139999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -1840,11 +1950,18 @@
         <v>75.610699999999994</v>
       </c>
       <c r="O17" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2368940669999997</v>
+      </c>
+      <c r="P17" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q17" s="16">
         <f t="shared" si="3"/>
-        <v>3.2368940669999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2920170099999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
@@ -1888,11 +2005,18 @@
         <v>77.304699999999997</v>
       </c>
       <c r="O18" s="21">
+        <f t="shared" si="4"/>
+        <v>3.3612083559999992</v>
+      </c>
+      <c r="P18" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q18" s="16">
         <f t="shared" si="3"/>
-        <v>3.3612083559999992</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2461952530000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>30</v>
       </c>
@@ -1936,11 +2060,18 @@
         <v>77.304699999999997</v>
       </c>
       <c r="O19" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2947263139999996</v>
+      </c>
+      <c r="P19" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q19" s="16">
         <f t="shared" si="3"/>
-        <v>3.2947263139999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.266993781</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>31</v>
       </c>
@@ -1984,11 +2115,18 @@
         <v>77.304699999999997</v>
       </c>
       <c r="O20" s="21">
+        <f t="shared" si="4"/>
+        <v>3.3179177239999995</v>
+      </c>
+      <c r="P20" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q20" s="16">
         <f t="shared" si="3"/>
-        <v>3.3179177239999995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2591943330000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>32</v>
       </c>
@@ -2032,11 +2170,18 @@
         <v>81.534199999999998</v>
       </c>
       <c r="O21" s="21">
+        <f t="shared" si="4"/>
+        <v>3.244245818</v>
+      </c>
+      <c r="P21" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q21" s="16">
         <f t="shared" si="3"/>
-        <v>3.244245818</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3056660440000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>34</v>
       </c>
@@ -2080,11 +2225,18 @@
         <v>81.534199999999998</v>
       </c>
       <c r="O22" s="21">
+        <f t="shared" si="4"/>
+        <v>3.3942687460000003</v>
+      </c>
+      <c r="P22" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q22" s="16">
         <f t="shared" si="3"/>
-        <v>3.3942687460000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.4977274510000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>35</v>
       </c>
@@ -2128,11 +2280,18 @@
         <v>81.534199999999998</v>
       </c>
       <c r="O23" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2450611599999997</v>
+      </c>
+      <c r="P23" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q23" s="16">
         <f t="shared" si="3"/>
-        <v>3.2450611599999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3193150780000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
@@ -2176,11 +2335,18 @@
         <v>82.914000000000001</v>
       </c>
       <c r="O24" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2717864400000001</v>
+      </c>
+      <c r="P24" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q24" s="16">
         <f t="shared" si="3"/>
-        <v>3.2717864400000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3482380310000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>38</v>
       </c>
@@ -2224,11 +2390,18 @@
         <v>82.914000000000001</v>
       </c>
       <c r="O25" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2029678200000005</v>
+      </c>
+      <c r="P25" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q25" s="16">
         <f t="shared" si="3"/>
-        <v>3.2029678200000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2257217020000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
@@ -2272,11 +2445,18 @@
         <v>82.914000000000001</v>
       </c>
       <c r="O26" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2344751399999998</v>
+      </c>
+      <c r="P26" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q26" s="16">
         <f t="shared" si="3"/>
-        <v>3.2344751399999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.266343827</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>40</v>
       </c>
@@ -2320,11 +2500,18 @@
         <v>93.764399999999995</v>
       </c>
       <c r="O27" s="21">
+        <f t="shared" si="4"/>
+        <v>3.3286362</v>
+      </c>
+      <c r="P27" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q27" s="16">
         <f t="shared" si="3"/>
-        <v>3.3286362</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2939668719999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>42</v>
       </c>
@@ -2368,11 +2555,18 @@
         <v>93.764399999999995</v>
       </c>
       <c r="O28" s="21">
+        <f t="shared" si="4"/>
+        <v>3.1589226359999998</v>
+      </c>
+      <c r="P28" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q28" s="16">
         <f t="shared" si="3"/>
-        <v>3.1589226359999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.260819218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>43</v>
       </c>
@@ -2416,11 +2610,18 @@
         <v>93.764399999999995</v>
       </c>
       <c r="O29" s="21">
+        <f t="shared" si="4"/>
+        <v>3.1504838400000001</v>
+      </c>
+      <c r="P29" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q29" s="16">
         <f t="shared" si="3"/>
-        <v>3.1504838400000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3631869729999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>44</v>
       </c>
@@ -2464,11 +2665,18 @@
         <v>107.4922</v>
       </c>
       <c r="O30" s="21">
+        <f t="shared" si="4"/>
+        <v>3.2054174039999999</v>
+      </c>
+      <c r="P30" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q30" s="16">
         <f t="shared" si="3"/>
-        <v>3.2054174039999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.295591757</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>46</v>
       </c>
@@ -2512,11 +2720,18 @@
         <v>107.4922</v>
       </c>
       <c r="O31" s="21">
+        <f t="shared" si="4"/>
+        <v>3.1989678719999999</v>
+      </c>
+      <c r="P31" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q31" s="16">
         <f t="shared" si="3"/>
-        <v>3.1989678719999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3339390430000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>47</v>
       </c>
@@ -2560,11 +2775,18 @@
         <v>107.4922</v>
       </c>
       <c r="O32" s="21">
+        <f t="shared" si="4"/>
+        <v>3.1559709919999999</v>
+      </c>
+      <c r="P32" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q32" s="16">
         <f t="shared" si="3"/>
-        <v>3.1559709919999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2578944249999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>48</v>
       </c>
@@ -2608,11 +2830,18 @@
         <v>1000</v>
       </c>
       <c r="O33" s="21">
+        <f t="shared" si="4"/>
+        <v>0.61</v>
+      </c>
+      <c r="P33" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q33" s="16">
         <f t="shared" si="3"/>
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.2715434590000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>50</v>
       </c>
@@ -2656,11 +2885,18 @@
         <v>1000</v>
       </c>
       <c r="O34" s="21">
+        <f t="shared" si="4"/>
+        <v>0.61</v>
+      </c>
+      <c r="P34" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q34" s="16">
         <f t="shared" si="3"/>
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.261469172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>51</v>
       </c>
@@ -2704,11 +2940,18 @@
         <v>1000</v>
       </c>
       <c r="O35" s="21">
+        <f t="shared" si="4"/>
+        <v>0.61</v>
+      </c>
+      <c r="P35" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q35" s="16">
         <f t="shared" si="3"/>
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3323141580000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>142</v>
       </c>
@@ -2752,11 +2995,18 @@
         <v>952</v>
       </c>
       <c r="O36" s="21">
+        <f t="shared" si="4"/>
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="P36" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q36" s="16">
         <f t="shared" si="3"/>
-        <v>0.95199999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.299491481</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>143</v>
       </c>
@@ -2800,11 +3050,18 @@
         <v>952</v>
       </c>
       <c r="O37" s="21">
+        <f t="shared" si="4"/>
+        <v>0.9329599999999999</v>
+      </c>
+      <c r="P37" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q37" s="16">
         <f t="shared" si="3"/>
-        <v>0.9329599999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3043661360000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>144</v>
       </c>
@@ -2848,8 +3105,15 @@
         <v>952</v>
       </c>
       <c r="O38" s="21">
+        <f t="shared" si="4"/>
+        <v>0.98055999999999999</v>
+      </c>
+      <c r="P38" s="16">
+        <v>32.497700000000002</v>
+      </c>
+      <c r="Q38" s="16">
         <f t="shared" si="3"/>
-        <v>0.98055999999999999</v>
+        <v>3.3423884450000001</v>
       </c>
     </row>
   </sheetData>
@@ -21754,10 +22018,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21993,6 +22257,20 @@
         <v>157</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>